<commit_message>
feat(pipelining): add text to the README about pipelining for the VonNeumann architecture #18
</commit_message>
<xml_diff>
--- a/programs/pipelining/fpumaclaurinprogramsinpiover2.xlsx
+++ b/programs/pipelining/fpumaclaurinprogramsinpiover2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vacla\Projects\cpu\programs\pipelining\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8BB8CE8-ADF1-4B81-9286-3C7E1C1D329B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63C12EF2-1EE8-4785-822A-1FA332A1A1C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E410B2C1-F054-41C4-A96D-F1120FBD95E0}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="100">
   <si>
     <t>Hex</t>
   </si>
@@ -236,12 +236,6 @@
   </si>
   <si>
     <t>should be 1</t>
-  </si>
-  <si>
-    <t>0x6e48</t>
-  </si>
-  <si>
-    <t>result from ISSIE</t>
   </si>
   <si>
     <t>calculate the partial resutl</t>
@@ -738,10 +732,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8E17FB6-AC76-4C3E-BEFA-6AB3607784FD}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Y35"/>
+  <dimension ref="A1:Y33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="K7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V24" sqref="V24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -993,7 +987,7 @@
       </c>
       <c r="H7" s="13"/>
       <c r="I7" s="13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J7" s="13"/>
       <c r="K7" s="1"/>
@@ -1011,10 +1005,10 @@
         <v>48</v>
       </c>
       <c r="U7" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="V7" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="W7" s="9"/>
       <c r="X7" s="8"/>
@@ -1022,7 +1016,7 @@
     </row>
     <row r="8" spans="1:25" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
@@ -1112,7 +1106,7 @@
         <v>55</v>
       </c>
       <c r="U9" s="10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.3">
@@ -1178,7 +1172,7 @@
         <v>56</v>
       </c>
       <c r="U10" s="10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="V10">
         <v>1.5703125</v>
@@ -1247,7 +1241,7 @@
         <v>57</v>
       </c>
       <c r="U11" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="V11">
         <v>0.1666259765625</v>
@@ -1316,7 +1310,7 @@
         <v>58</v>
       </c>
       <c r="U12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="V12">
         <v>0.260498046875</v>
@@ -1385,7 +1379,7 @@
         <v>58</v>
       </c>
       <c r="U13" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="V13">
         <v>0.40966796875</v>
@@ -1454,7 +1448,7 @@
         <v>58</v>
       </c>
       <c r="U14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="V14">
         <v>0.64208984375</v>
@@ -1523,7 +1517,7 @@
         <v>62</v>
       </c>
       <c r="U15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="V15">
         <v>0.9287109375</v>
@@ -1652,7 +1646,7 @@
         <v>60</v>
       </c>
       <c r="U17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.3">
@@ -1718,7 +1712,7 @@
         <v>58</v>
       </c>
       <c r="U18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.3">
@@ -1784,7 +1778,7 @@
         <v>58</v>
       </c>
       <c r="U19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.3">
@@ -1850,7 +1844,7 @@
         <v>58</v>
       </c>
       <c r="U20" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.3">
@@ -1916,7 +1910,7 @@
         <v>58</v>
       </c>
       <c r="U21" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.3">
@@ -1982,7 +1976,7 @@
         <v>58</v>
       </c>
       <c r="U22" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.3">
@@ -2048,10 +2042,10 @@
         <v>53</v>
       </c>
       <c r="U23" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="V23">
-        <v>1.0045248600000001</v>
+        <v>0.99462890999999998</v>
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.3">
@@ -2176,7 +2170,7 @@
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A26" s="13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B26" s="13"/>
       <c r="C26" s="13"/>
@@ -2325,7 +2319,7 @@
         <v>65</v>
       </c>
       <c r="T29" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.3">
@@ -2455,71 +2449,15 @@
         <v>1400</v>
       </c>
       <c r="T32" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>64</v>
       </c>
       <c r="T33" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>68</v>
-      </c>
-      <c r="B35" t="s">
-        <v>67</v>
-      </c>
-      <c r="C35">
-        <v>0</v>
-      </c>
-      <c r="D35">
-        <v>1</v>
-      </c>
-      <c r="E35">
-        <v>1</v>
-      </c>
-      <c r="F35">
-        <v>0</v>
-      </c>
-      <c r="G35">
-        <v>1</v>
-      </c>
-      <c r="H35">
-        <v>1</v>
-      </c>
-      <c r="I35">
-        <v>1</v>
-      </c>
-      <c r="J35">
-        <v>0</v>
-      </c>
-      <c r="K35">
-        <v>0</v>
-      </c>
-      <c r="L35">
-        <v>1</v>
-      </c>
-      <c r="M35">
-        <v>0</v>
-      </c>
-      <c r="N35">
-        <v>0</v>
-      </c>
-      <c r="O35">
-        <v>1</v>
-      </c>
-      <c r="P35">
-        <v>0</v>
-      </c>
-      <c r="Q35">
-        <v>0</v>
-      </c>
-      <c r="R35">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2529,6 +2467,11 @@
     <mergeCell ref="I6:J6"/>
     <mergeCell ref="Q6:R6"/>
     <mergeCell ref="K6:P6"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="I5:R5"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="G6:H6"/>
     <mergeCell ref="C7:F7"/>
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="I7:J7"/>
@@ -2543,11 +2486,6 @@
     <mergeCell ref="K3:N3"/>
     <mergeCell ref="O3:P3"/>
     <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="I5:R5"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="G6:H6"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2560,7 +2498,7 @@
   <dimension ref="A1:AK21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2680,19 +2618,19 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C2" t="s">
         <v>23</v>
       </c>
       <c r="D2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F2" t="s">
         <v>89</v>
-      </c>
-      <c r="E2" t="s">
-        <v>90</v>
-      </c>
-      <c r="F2" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.3">
@@ -2700,22 +2638,22 @@
         <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>40</v>
       </c>
       <c r="E3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G3" t="s">
+        <v>88</v>
+      </c>
+      <c r="H3" t="s">
         <v>89</v>
-      </c>
-      <c r="G3" t="s">
-        <v>90</v>
-      </c>
-      <c r="H3" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.3">
@@ -2723,22 +2661,22 @@
         <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C4" t="s">
         <v>24</v>
       </c>
       <c r="G4" t="s">
+        <v>87</v>
+      </c>
+      <c r="H4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I4" t="s">
+        <v>88</v>
+      </c>
+      <c r="J4" t="s">
         <v>89</v>
-      </c>
-      <c r="H4" t="s">
-        <v>92</v>
-      </c>
-      <c r="I4" t="s">
-        <v>90</v>
-      </c>
-      <c r="J4" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.3">
@@ -2746,22 +2684,22 @@
         <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>54</v>
       </c>
       <c r="I5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J5" t="s">
+        <v>87</v>
+      </c>
+      <c r="K5" t="s">
+        <v>88</v>
+      </c>
+      <c r="L5" t="s">
         <v>89</v>
-      </c>
-      <c r="K5" t="s">
-        <v>90</v>
-      </c>
-      <c r="L5" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.3">
@@ -2769,22 +2707,22 @@
         <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>54</v>
       </c>
       <c r="K6" t="s">
+        <v>87</v>
+      </c>
+      <c r="L6" t="s">
+        <v>90</v>
+      </c>
+      <c r="M6" t="s">
+        <v>88</v>
+      </c>
+      <c r="N6" t="s">
         <v>89</v>
-      </c>
-      <c r="L6" t="s">
-        <v>92</v>
-      </c>
-      <c r="M6" t="s">
-        <v>90</v>
-      </c>
-      <c r="N6" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.3">
@@ -2792,22 +2730,22 @@
         <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>54</v>
       </c>
       <c r="M7" t="s">
+        <v>87</v>
+      </c>
+      <c r="N7" t="s">
+        <v>90</v>
+      </c>
+      <c r="O7" t="s">
+        <v>88</v>
+      </c>
+      <c r="P7" t="s">
         <v>89</v>
-      </c>
-      <c r="N7" t="s">
-        <v>92</v>
-      </c>
-      <c r="O7" t="s">
-        <v>90</v>
-      </c>
-      <c r="P7" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.3">
@@ -2815,19 +2753,19 @@
         <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C8" t="s">
         <v>61</v>
       </c>
       <c r="O8" t="s">
+        <v>87</v>
+      </c>
+      <c r="P8" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q8" t="s">
         <v>89</v>
-      </c>
-      <c r="P8" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.3">
@@ -2835,22 +2773,22 @@
         <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C9" t="s">
         <v>47</v>
       </c>
       <c r="P9" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>90</v>
+      </c>
+      <c r="R9" t="s">
+        <v>88</v>
+      </c>
+      <c r="S9" t="s">
         <v>89</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>92</v>
-      </c>
-      <c r="R9" t="s">
-        <v>90</v>
-      </c>
-      <c r="S9" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.3">
@@ -2858,22 +2796,22 @@
         <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C10" t="s">
         <v>24</v>
       </c>
       <c r="R10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="S10" t="s">
+        <v>87</v>
+      </c>
+      <c r="T10" t="s">
+        <v>88</v>
+      </c>
+      <c r="U10" t="s">
         <v>89</v>
-      </c>
-      <c r="T10" t="s">
-        <v>90</v>
-      </c>
-      <c r="U10" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.3">
@@ -2881,22 +2819,22 @@
         <v>34</v>
       </c>
       <c r="B11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C11" t="s">
         <v>54</v>
       </c>
       <c r="T11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="U11" t="s">
+        <v>87</v>
+      </c>
+      <c r="V11" t="s">
+        <v>88</v>
+      </c>
+      <c r="W11" t="s">
         <v>89</v>
-      </c>
-      <c r="V11" t="s">
-        <v>90</v>
-      </c>
-      <c r="W11" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.3">
@@ -2904,22 +2842,22 @@
         <v>41</v>
       </c>
       <c r="B12" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C12" t="s">
         <v>54</v>
       </c>
       <c r="V12" t="s">
+        <v>87</v>
+      </c>
+      <c r="W12" t="s">
+        <v>90</v>
+      </c>
+      <c r="X12" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y12" t="s">
         <v>89</v>
-      </c>
-      <c r="W12" t="s">
-        <v>92</v>
-      </c>
-      <c r="X12" t="s">
-        <v>90</v>
-      </c>
-      <c r="Y12" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.3">
@@ -2927,22 +2865,22 @@
         <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C13" t="s">
         <v>54</v>
       </c>
       <c r="X13" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>90</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA13" t="s">
         <v>89</v>
-      </c>
-      <c r="Y13" t="s">
-        <v>92</v>
-      </c>
-      <c r="Z13" t="s">
-        <v>90</v>
-      </c>
-      <c r="AA13" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.3">
@@ -2950,22 +2888,22 @@
         <v>43</v>
       </c>
       <c r="B14" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C14" t="s">
         <v>54</v>
       </c>
       <c r="Z14" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>88</v>
+      </c>
+      <c r="AC14" t="s">
         <v>89</v>
-      </c>
-      <c r="AA14" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB14" t="s">
-        <v>90</v>
-      </c>
-      <c r="AC14" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.3">
@@ -2973,22 +2911,22 @@
         <v>44</v>
       </c>
       <c r="B15" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C15" t="s">
         <v>54</v>
       </c>
       <c r="AB15" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>90</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>88</v>
+      </c>
+      <c r="AE15" t="s">
         <v>89</v>
-      </c>
-      <c r="AC15" t="s">
-        <v>92</v>
-      </c>
-      <c r="AD15" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE15" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.3">
@@ -2996,19 +2934,19 @@
         <v>45</v>
       </c>
       <c r="B16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C16" t="s">
         <v>59</v>
       </c>
       <c r="AD16" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>88</v>
+      </c>
+      <c r="AF16" t="s">
         <v>89</v>
-      </c>
-      <c r="AE16" t="s">
-        <v>90</v>
-      </c>
-      <c r="AF16" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:36" x14ac:dyDescent="0.3">
@@ -3016,22 +2954,22 @@
         <v>46</v>
       </c>
       <c r="B17" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C17" t="s">
         <v>47</v>
       </c>
       <c r="AE17" t="s">
+        <v>87</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>90</v>
+      </c>
+      <c r="AG17" t="s">
+        <v>88</v>
+      </c>
+      <c r="AH17" t="s">
         <v>89</v>
-      </c>
-      <c r="AF17" t="s">
-        <v>92</v>
-      </c>
-      <c r="AG17" t="s">
-        <v>90</v>
-      </c>
-      <c r="AH17" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:36" x14ac:dyDescent="0.3">
@@ -3039,27 +2977,27 @@
         <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C18" t="s">
         <v>63</v>
       </c>
       <c r="AG18" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="AH18" t="s">
+        <v>87</v>
+      </c>
+      <c r="AI18" t="s">
+        <v>88</v>
+      </c>
+      <c r="AJ18" t="s">
         <v>89</v>
-      </c>
-      <c r="AI18" t="s">
-        <v>90</v>
-      </c>
-      <c r="AJ18" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:36" x14ac:dyDescent="0.3">
       <c r="D21" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(pipelining): fix the pipelining for the Harvard architecture #18
</commit_message>
<xml_diff>
--- a/programs/pipelining/fpumaclaurinprogramsinpiover2.xlsx
+++ b/programs/pipelining/fpumaclaurinprogramsinpiover2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vacla\Projects\cpu\programs\pipelining\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63C12EF2-1EE8-4785-822A-1FA332A1A1C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11817379-B5F3-4CD4-AA60-FAE8AB869430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E410B2C1-F054-41C4-A96D-F1120FBD95E0}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="95">
   <si>
     <t>Hex</t>
   </si>
@@ -310,31 +310,16 @@
     <t>ST</t>
   </si>
   <si>
-    <t>Problematic cycle in which the STALL out will not be generated but because there is a reg hazard, then the IR1 will be stored, therefore using STALL_PREV_PREV</t>
-  </si>
-  <si>
-    <t>744</t>
-  </si>
-  <si>
-    <t>CC01</t>
-  </si>
-  <si>
-    <t>B44</t>
-  </si>
-  <si>
-    <t>1A01</t>
-  </si>
-  <si>
-    <t>1D02</t>
-  </si>
-  <si>
-    <t>D44</t>
-  </si>
-  <si>
-    <t>1C02</t>
-  </si>
-  <si>
-    <t>7000</t>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Instruction</t>
+  </si>
+  <si>
+    <t>Clock cycles</t>
   </si>
 </sst>
 </file>
@@ -734,8 +719,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Y33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V24" sqref="V24"/>
+    <sheetView tabSelected="1" topLeftCell="H16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U23" sqref="U23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2495,512 +2480,580 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD75EAF5-2CFE-4CF5-ACF9-EFC0B7AB3B75}">
-  <dimension ref="A1:AK21"/>
+  <dimension ref="A1:AH19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" customWidth="1"/>
     <col min="4" max="36" width="4.6640625" customWidth="1"/>
     <col min="37" max="37" width="4.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="D1">
-        <v>0</v>
-      </c>
-      <c r="E1">
-        <v>1</v>
-      </c>
-      <c r="F1">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="13"/>
+      <c r="W1" s="13"/>
+      <c r="X1" s="13"/>
+      <c r="Y1" s="13"/>
+      <c r="Z1" s="13"/>
+      <c r="AA1" s="13"/>
+      <c r="AB1" s="13"/>
+      <c r="AC1" s="13"/>
+      <c r="AD1" s="13"/>
+      <c r="AE1" s="13"/>
+      <c r="AF1" s="13"/>
+      <c r="AG1" s="13"/>
+      <c r="AH1" s="13"/>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
         <v>2</v>
       </c>
-      <c r="G1">
+      <c r="G2">
         <v>3</v>
       </c>
-      <c r="H1">
+      <c r="H2">
         <v>4</v>
       </c>
-      <c r="I1">
+      <c r="I2">
         <v>5</v>
       </c>
-      <c r="J1">
+      <c r="J2">
         <v>6</v>
       </c>
-      <c r="K1">
+      <c r="K2">
         <v>7</v>
       </c>
-      <c r="L1">
+      <c r="L2">
         <v>8</v>
       </c>
-      <c r="M1">
+      <c r="M2">
         <v>9</v>
       </c>
-      <c r="N1">
+      <c r="N2">
         <v>10</v>
       </c>
-      <c r="O1">
+      <c r="O2">
         <v>11</v>
       </c>
-      <c r="P1">
+      <c r="P2">
         <v>12</v>
       </c>
-      <c r="Q1">
+      <c r="Q2">
         <v>13</v>
       </c>
-      <c r="R1">
+      <c r="R2">
         <v>14</v>
       </c>
-      <c r="S1">
+      <c r="S2">
         <v>15</v>
       </c>
-      <c r="T1">
+      <c r="T2">
         <v>16</v>
       </c>
-      <c r="U1">
+      <c r="U2">
         <v>17</v>
       </c>
-      <c r="V1">
+      <c r="V2">
         <v>18</v>
       </c>
-      <c r="W1">
+      <c r="W2">
         <v>19</v>
       </c>
-      <c r="X1">
+      <c r="X2">
         <v>20</v>
       </c>
-      <c r="Y1">
+      <c r="Y2">
         <v>21</v>
       </c>
-      <c r="Z1">
+      <c r="Z2">
         <v>22</v>
       </c>
-      <c r="AA1">
+      <c r="AA2">
         <v>23</v>
       </c>
-      <c r="AB1">
+      <c r="AB2">
         <v>24</v>
       </c>
-      <c r="AC1">
+      <c r="AC2">
         <v>25</v>
       </c>
-      <c r="AD1">
+      <c r="AD2">
         <v>26</v>
       </c>
-      <c r="AE1">
+      <c r="AE2">
         <v>27</v>
       </c>
-      <c r="AF1">
+      <c r="AF2">
         <v>28</v>
       </c>
-      <c r="AG1">
+      <c r="AG2">
         <v>29</v>
       </c>
-      <c r="AH1">
+      <c r="AH2">
         <v>30</v>
       </c>
-      <c r="AI1">
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="str">
+        <f>Code!B9</f>
+        <v>LDR R1, [R0], #1</v>
+      </c>
+      <c r="C3" t="str">
+        <f>Code!S9</f>
+        <v>744</v>
+      </c>
+      <c r="D3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="str">
+        <f>Code!B10</f>
+        <v>MOV R3 = R1 LSL #0</v>
+      </c>
+      <c r="C4" t="str">
+        <f>Code!S10</f>
+        <v>CC01</v>
+      </c>
+      <c r="E4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="str">
+        <f>Code!B11</f>
+        <v>LDR R2, [R0], #1</v>
+      </c>
+      <c r="C5" t="str">
+        <f>Code!S11</f>
+        <v>B44</v>
+      </c>
+      <c r="F5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H5" t="s">
+        <v>88</v>
+      </c>
+      <c r="I5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="str">
+        <f>Code!B12</f>
+        <v>FMUL R2, R1</v>
+      </c>
+      <c r="C6" t="str">
+        <f>Code!S12</f>
+        <v>1A01</v>
+      </c>
+      <c r="H6" t="s">
+        <v>87</v>
+      </c>
+      <c r="I6" t="s">
+        <v>90</v>
+      </c>
+      <c r="J6" t="s">
+        <v>88</v>
+      </c>
+      <c r="K6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" t="str">
+        <f>Code!B13</f>
+        <v>FMUL R2, R1</v>
+      </c>
+      <c r="C7" t="str">
+        <f>Code!S13</f>
+        <v>1A01</v>
+      </c>
+      <c r="J7" t="s">
+        <v>87</v>
+      </c>
+      <c r="K7" t="s">
+        <v>90</v>
+      </c>
+      <c r="L7" t="s">
+        <v>88</v>
+      </c>
+      <c r="M7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" t="str">
+        <f>Code!B14</f>
+        <v>FMUL R2, R1</v>
+      </c>
+      <c r="C8" t="str">
+        <f>Code!S14</f>
+        <v>1A01</v>
+      </c>
+      <c r="L8" t="s">
+        <v>87</v>
+      </c>
+      <c r="M8" t="s">
+        <v>90</v>
+      </c>
+      <c r="N8" t="s">
+        <v>88</v>
+      </c>
+      <c r="O8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>31</v>
       </c>
-      <c r="AJ1">
+      <c r="B9" t="str">
+        <f>Code!B15</f>
+        <v>FSUB R3, R2</v>
+      </c>
+      <c r="C9" t="str">
+        <f>Code!S15</f>
+        <v>1D02</v>
+      </c>
+      <c r="N9" t="s">
+        <v>87</v>
+      </c>
+      <c r="O9" t="s">
+        <v>88</v>
+      </c>
+      <c r="P9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>32</v>
       </c>
-      <c r="AK1">
+      <c r="B10" t="str">
+        <f>Code!B16</f>
+        <v>STR R3, [R0], #1</v>
+      </c>
+      <c r="C10" t="str">
+        <f>Code!S16</f>
+        <v>D44</v>
+      </c>
+      <c r="O10" t="s">
+        <v>87</v>
+      </c>
+      <c r="P10" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>88</v>
+      </c>
+      <c r="R10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B11" t="str">
+        <f>Code!B17</f>
+        <v>LDR R2, [R0], #1</v>
+      </c>
+      <c r="C11" t="str">
+        <f>Code!S17</f>
+        <v>B44</v>
+      </c>
+      <c r="Q11" t="s">
         <v>87</v>
       </c>
-      <c r="E2" t="s">
+      <c r="R11" t="s">
+        <v>90</v>
+      </c>
+      <c r="S11" t="s">
         <v>88</v>
       </c>
-      <c r="F2" t="s">
+      <c r="T11" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E3" t="s">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" t="str">
+        <f>Code!B18</f>
+        <v>FMUL R2, R1</v>
+      </c>
+      <c r="C12" t="str">
+        <f>Code!S18</f>
+        <v>1A01</v>
+      </c>
+      <c r="S12" t="s">
+        <v>87</v>
+      </c>
+      <c r="T12" t="s">
         <v>90</v>
       </c>
-      <c r="F3" t="s">
+      <c r="U12" t="s">
+        <v>88</v>
+      </c>
+      <c r="V12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="str">
+        <f>Code!B19</f>
+        <v>FMUL R2, R1</v>
+      </c>
+      <c r="C13" t="str">
+        <f>Code!S19</f>
+        <v>1A01</v>
+      </c>
+      <c r="U13" t="s">
         <v>87</v>
       </c>
-      <c r="G3" t="s">
+      <c r="V13" t="s">
+        <v>90</v>
+      </c>
+      <c r="W13" t="s">
         <v>88</v>
       </c>
-      <c r="H3" t="s">
+      <c r="X13" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" t="s">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" t="str">
+        <f>Code!B20</f>
+        <v>FMUL R2, R1</v>
+      </c>
+      <c r="C14" t="str">
+        <f>Code!S20</f>
+        <v>1A01</v>
+      </c>
+      <c r="W14" t="s">
         <v>87</v>
       </c>
-      <c r="H4" t="s">
+      <c r="X14" t="s">
         <v>90</v>
       </c>
-      <c r="I4" t="s">
+      <c r="Y14" t="s">
         <v>88</v>
       </c>
-      <c r="J4" t="s">
+      <c r="Z14" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="I5" t="s">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" t="str">
+        <f>Code!B21</f>
+        <v>FMUL R2, R1</v>
+      </c>
+      <c r="C15" t="str">
+        <f>Code!S21</f>
+        <v>1A01</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z15" t="s">
         <v>90</v>
       </c>
-      <c r="J5" t="s">
+      <c r="AA15" t="s">
+        <v>88</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" t="str">
+        <f>Code!B22</f>
+        <v>FMUL R2, R1</v>
+      </c>
+      <c r="C16" t="str">
+        <f>Code!S22</f>
+        <v>1A01</v>
+      </c>
+      <c r="AA16" t="s">
         <v>87</v>
       </c>
-      <c r="K5" t="s">
+      <c r="AB16" t="s">
+        <v>90</v>
+      </c>
+      <c r="AC16" t="s">
         <v>88</v>
       </c>
-      <c r="L5" t="s">
+      <c r="AD16" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" t="s">
-        <v>95</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="K6" t="s">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" t="str">
+        <f>Code!B23</f>
+        <v>FADD R3, R2</v>
+      </c>
+      <c r="C17" t="str">
+        <f>Code!S23</f>
+        <v>1C02</v>
+      </c>
+      <c r="AC17" t="s">
         <v>87</v>
       </c>
-      <c r="L6" t="s">
+      <c r="AD17" t="s">
+        <v>88</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" t="str">
+        <f>Code!B24</f>
+        <v>STR R3, [R0], #1</v>
+      </c>
+      <c r="C18" t="str">
+        <f>Code!S24</f>
+        <v>D44</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE18" t="s">
         <v>90</v>
       </c>
-      <c r="M6" t="s">
+      <c r="AF18" t="s">
         <v>88</v>
       </c>
-      <c r="N6" t="s">
+      <c r="AG18" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" t="s">
-        <v>95</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="M7" t="s">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" t="str">
+        <f>Code!B25</f>
+        <v>STP</v>
+      </c>
+      <c r="C19" t="str">
+        <f>Code!S25</f>
+        <v>7000</v>
+      </c>
+      <c r="AF19" t="s">
         <v>87</v>
       </c>
-      <c r="N7" t="s">
-        <v>90</v>
-      </c>
-      <c r="O7" t="s">
+      <c r="AG19" t="s">
         <v>88</v>
       </c>
-      <c r="P7" t="s">
+      <c r="AH19" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" t="s">
-        <v>96</v>
-      </c>
-      <c r="C8" t="s">
-        <v>61</v>
-      </c>
-      <c r="O8" t="s">
-        <v>87</v>
-      </c>
-      <c r="P8" t="s">
-        <v>88</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" t="s">
-        <v>97</v>
-      </c>
-      <c r="C9" t="s">
-        <v>47</v>
-      </c>
-      <c r="P9" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>90</v>
-      </c>
-      <c r="R9" t="s">
-        <v>88</v>
-      </c>
-      <c r="S9" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" t="s">
-        <v>94</v>
-      </c>
-      <c r="C10" t="s">
-        <v>24</v>
-      </c>
-      <c r="R10" t="s">
-        <v>90</v>
-      </c>
-      <c r="S10" t="s">
-        <v>87</v>
-      </c>
-      <c r="T10" t="s">
-        <v>88</v>
-      </c>
-      <c r="U10" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" t="s">
-        <v>95</v>
-      </c>
-      <c r="C11" t="s">
-        <v>54</v>
-      </c>
-      <c r="T11" t="s">
-        <v>90</v>
-      </c>
-      <c r="U11" t="s">
-        <v>87</v>
-      </c>
-      <c r="V11" t="s">
-        <v>88</v>
-      </c>
-      <c r="W11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" t="s">
-        <v>95</v>
-      </c>
-      <c r="C12" t="s">
-        <v>54</v>
-      </c>
-      <c r="V12" t="s">
-        <v>87</v>
-      </c>
-      <c r="W12" t="s">
-        <v>90</v>
-      </c>
-      <c r="X12" t="s">
-        <v>88</v>
-      </c>
-      <c r="Y12" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" t="s">
-        <v>95</v>
-      </c>
-      <c r="C13" t="s">
-        <v>54</v>
-      </c>
-      <c r="X13" t="s">
-        <v>87</v>
-      </c>
-      <c r="Y13" t="s">
-        <v>90</v>
-      </c>
-      <c r="Z13" t="s">
-        <v>88</v>
-      </c>
-      <c r="AA13" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" t="s">
-        <v>95</v>
-      </c>
-      <c r="C14" t="s">
-        <v>54</v>
-      </c>
-      <c r="Z14" t="s">
-        <v>87</v>
-      </c>
-      <c r="AA14" t="s">
-        <v>90</v>
-      </c>
-      <c r="AB14" t="s">
-        <v>88</v>
-      </c>
-      <c r="AC14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>44</v>
-      </c>
-      <c r="B15" t="s">
-        <v>95</v>
-      </c>
-      <c r="C15" t="s">
-        <v>54</v>
-      </c>
-      <c r="AB15" t="s">
-        <v>87</v>
-      </c>
-      <c r="AC15" t="s">
-        <v>90</v>
-      </c>
-      <c r="AD15" t="s">
-        <v>88</v>
-      </c>
-      <c r="AE15" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>45</v>
-      </c>
-      <c r="B16" t="s">
-        <v>98</v>
-      </c>
-      <c r="C16" t="s">
-        <v>59</v>
-      </c>
-      <c r="AD16" t="s">
-        <v>87</v>
-      </c>
-      <c r="AE16" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF16" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>46</v>
-      </c>
-      <c r="B17" t="s">
-        <v>97</v>
-      </c>
-      <c r="C17" t="s">
-        <v>47</v>
-      </c>
-      <c r="AE17" t="s">
-        <v>87</v>
-      </c>
-      <c r="AF17" t="s">
-        <v>90</v>
-      </c>
-      <c r="AG17" t="s">
-        <v>88</v>
-      </c>
-      <c r="AH17" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" t="s">
-        <v>99</v>
-      </c>
-      <c r="C18" t="s">
-        <v>63</v>
-      </c>
-      <c r="AG18" t="s">
-        <v>90</v>
-      </c>
-      <c r="AH18" t="s">
-        <v>87</v>
-      </c>
-      <c r="AI18" t="s">
-        <v>88</v>
-      </c>
-      <c r="AJ18" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="D21" t="s">
-        <v>91</v>
-      </c>
-    </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:AH1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix(fpu-32-bits): fix FPU multiplication of following FMUL instructions #2
</commit_message>
<xml_diff>
--- a/programs/pipelining/fpumaclaurinprogramsinpiover2.xlsx
+++ b/programs/pipelining/fpumaclaurinprogramsinpiover2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vacla\Projects\cpu\programs\pipelining\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11817379-B5F3-4CD4-AA60-FAE8AB869430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66803C3B-1AF0-4420-90AA-4AD4E8C79974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E410B2C1-F054-41C4-A96D-F1120FBD95E0}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{E410B2C1-F054-41C4-A96D-F1120FBD95E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Code" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="140">
   <si>
     <t>Hex</t>
   </si>
@@ -320,6 +320,141 @@
   </si>
   <si>
     <t>Clock cycles</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>correct answer</t>
+  </si>
+  <si>
+    <t>010000101111101111010000000000</t>
+  </si>
+  <si>
+    <t>ISSIE multiplication based on the single precission</t>
+  </si>
+  <si>
+    <t>0x342f</t>
+  </si>
+  <si>
+    <t>0x3691</t>
+  </si>
+  <si>
+    <t>0x3927</t>
+  </si>
+  <si>
+    <t>0x2040</t>
+  </si>
+  <si>
+    <t>0x22ac</t>
+  </si>
+  <si>
+    <t>0x253d</t>
+  </si>
+  <si>
+    <t>0x281c</t>
+  </si>
+  <si>
+    <t>0x2a73</t>
+  </si>
+  <si>
+    <t>0x2d10</t>
+  </si>
+  <si>
+    <t>0x3005</t>
+  </si>
+  <si>
+    <t>0x3b69</t>
+  </si>
+  <si>
+    <t>0x1c02</t>
+  </si>
+  <si>
+    <t>Addition</t>
+  </si>
+  <si>
+    <t>resultant mantissa</t>
+  </si>
+  <si>
+    <t>E-7-02</t>
+  </si>
+  <si>
+    <t>result of the addition</t>
+  </si>
+  <si>
+    <t>ISSIE after zeroing bits</t>
+  </si>
+  <si>
+    <t>0x342b</t>
+  </si>
+  <si>
+    <t>0x3686</t>
+  </si>
+  <si>
+    <t>0x391d</t>
+  </si>
+  <si>
+    <t>0x3b73</t>
+  </si>
+  <si>
+    <t>0x224b</t>
+  </si>
+  <si>
+    <t>0x24b6</t>
+  </si>
+  <si>
+    <t>0x297f</t>
+  </si>
+  <si>
+    <t>0x2c38</t>
+  </si>
+  <si>
+    <t>0x2ffa</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>3155 mantissa</t>
+  </si>
+  <si>
+    <t>3e48 mantissa</t>
+  </si>
+  <si>
+    <t>OP1 mantissa</t>
+  </si>
+  <si>
+    <t>OP2 mantissa</t>
+  </si>
+  <si>
+    <t>second multiplication</t>
+  </si>
+  <si>
+    <t>op2 mantissa</t>
+  </si>
+  <si>
+    <t>0x3e48</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>1A1B40000000</t>
+  </si>
+  <si>
+    <t>resultant mantissa after the second multiplication</t>
+  </si>
+  <si>
+    <t>check the addition</t>
+  </si>
+  <si>
+    <t>compare the multiplication with one from online</t>
+  </si>
+  <si>
+    <t>encoded result</t>
+  </si>
+  <si>
+    <t>e</t>
   </si>
 </sst>
 </file>
@@ -357,7 +492,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -365,11 +500,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -389,9 +542,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -399,9 +549,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -717,24 +881,24 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8E17FB6-AC76-4C3E-BEFA-6AB3607784FD}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Y33"/>
+  <dimension ref="A1:Y101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U23" sqref="U23"/>
+    <sheetView tabSelected="1" topLeftCell="A87" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D96" sqref="D96"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" customWidth="1"/>
-    <col min="2" max="2" width="22.77734375" customWidth="1"/>
-    <col min="20" max="20" width="22.88671875" customWidth="1"/>
-    <col min="21" max="21" width="19.6640625" customWidth="1"/>
-    <col min="22" max="22" width="18.5546875" customWidth="1"/>
-    <col min="23" max="23" width="30.33203125" customWidth="1"/>
-    <col min="24" max="24" width="27.88671875" customWidth="1"/>
+    <col min="1" max="1" width="17.3125" customWidth="1"/>
+    <col min="2" max="2" width="22.7890625" customWidth="1"/>
+    <col min="20" max="20" width="22.89453125" customWidth="1"/>
+    <col min="21" max="21" width="19.68359375" customWidth="1"/>
+    <col min="22" max="22" width="18.5234375" customWidth="1"/>
+    <col min="23" max="23" width="30.3125" customWidth="1"/>
+    <col min="24" max="24" width="27.89453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="C1">
         <v>15</v>
       </c>
@@ -784,79 +948,79 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13" t="s">
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="13"/>
+      <c r="H2" s="15"/>
       <c r="I2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13" t="s">
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13" t="s">
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="13"/>
+      <c r="H3" s="15"/>
       <c r="I3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="K3" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13" t="s">
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="13" t="s">
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="R3" s="13"/>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="R3" s="15"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" t="s">
         <v>13</v>
       </c>
@@ -872,10 +1036,10 @@
       <c r="F4" s="1">
         <v>0</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="13"/>
+      <c r="H4" s="15"/>
       <c r="I4" s="1" t="s">
         <v>14</v>
       </c>
@@ -888,93 +1052,93 @@
       <c r="L4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="13" t="s">
+      <c r="M4" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="13" t="s">
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="R4" s="13"/>
-    </row>
-    <row r="5" spans="1:25" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R4" s="15"/>
+    </row>
+    <row r="5" spans="1:25" ht="11.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13" t="s">
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="13"/>
-      <c r="R5" s="13"/>
-    </row>
-    <row r="6" spans="1:25" ht="13.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="15"/>
+    </row>
+    <row r="6" spans="1:25" ht="13.2" hidden="1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13" t="s">
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13" t="s">
+      <c r="H6" s="15"/>
+      <c r="I6" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13" t="s">
+      <c r="J6" s="15"/>
+      <c r="K6" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="13" t="s">
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="R6" s="13"/>
-    </row>
-    <row r="7" spans="1:25" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R6" s="15"/>
+    </row>
+    <row r="7" spans="1:25" ht="63.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13" t="s">
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13" t="s">
+      <c r="H7" s="15"/>
+      <c r="I7" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="J7" s="13"/>
+      <c r="J7" s="15"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
@@ -995,40 +1159,46 @@
       <c r="V7" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="W7" s="9"/>
-      <c r="X7" s="8"/>
-      <c r="Y7" s="8"/>
-    </row>
-    <row r="8" spans="1:25" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="13" t="s">
+      <c r="W7" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="X7" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y7" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" ht="13.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="13"/>
-      <c r="P8" s="13"/>
-      <c r="Q8" s="13"/>
-      <c r="R8" s="13"/>
-      <c r="S8" s="13"/>
-      <c r="T8" s="13"/>
-      <c r="U8" s="13"/>
-      <c r="V8" s="13"/>
-      <c r="W8" s="12"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="15"/>
+      <c r="S8" s="15"/>
+      <c r="T8" s="15"/>
+      <c r="U8" s="15"/>
+      <c r="V8" s="15"/>
+      <c r="W8" s="11"/>
       <c r="X8" s="8"/>
       <c r="Y8" s="8"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -1090,11 +1260,11 @@
       <c r="T9" t="s">
         <v>55</v>
       </c>
-      <c r="U9" s="10" t="s">
+      <c r="U9" s="9" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1156,14 +1326,14 @@
       <c r="T10" t="s">
         <v>56</v>
       </c>
-      <c r="U10" s="10" t="s">
+      <c r="U10" s="9" t="s">
         <v>70</v>
       </c>
       <c r="V10">
         <v>1.5703125</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1225,14 +1395,14 @@
       <c r="T11" t="s">
         <v>57</v>
       </c>
-      <c r="U11" s="11" t="s">
+      <c r="U11" s="10" t="s">
         <v>79</v>
       </c>
       <c r="V11">
         <v>0.1666259765625</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -1300,8 +1470,14 @@
       <c r="V12">
         <v>0.260498046875</v>
       </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="W12" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -1369,8 +1545,14 @@
       <c r="V13">
         <v>0.40966796875</v>
       </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="W13" t="s">
+        <v>100</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -1438,8 +1620,14 @@
       <c r="V14">
         <v>0.64208984375</v>
       </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="W14" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -1507,8 +1695,14 @@
       <c r="V15">
         <v>0.9287109375</v>
       </c>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="W15" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1568,7 +1762,7 @@
         <v>D44</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -1633,8 +1827,14 @@
       <c r="U17" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W17" t="s">
+        <v>102</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -1699,8 +1899,14 @@
       <c r="U18" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W18" t="s">
+        <v>103</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>41</v>
       </c>
@@ -1765,8 +1971,14 @@
       <c r="U19" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W19" t="s">
+        <v>104</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>42</v>
       </c>
@@ -1831,8 +2043,14 @@
       <c r="U20" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W20" t="s">
+        <v>105</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -1897,8 +2115,14 @@
       <c r="U21" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W21" t="s">
+        <v>106</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>44</v>
       </c>
@@ -1963,8 +2187,14 @@
       <c r="U22" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W22" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>45</v>
       </c>
@@ -2032,8 +2262,14 @@
       <c r="V23">
         <v>0.99462890999999998</v>
       </c>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W23" t="s">
+        <v>108</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -2093,7 +2329,7 @@
         <v>D44</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -2153,30 +2389,30 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A26" s="13" t="s">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="13"/>
-      <c r="K26" s="13"/>
-      <c r="L26" s="13"/>
-      <c r="M26" s="13"/>
-      <c r="N26" s="13"/>
-      <c r="O26" s="13"/>
-      <c r="P26" s="13"/>
-      <c r="Q26" s="13"/>
-      <c r="R26" s="13"/>
-      <c r="S26" s="13"/>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="15"/>
+      <c r="K26" s="15"/>
+      <c r="L26" s="15"/>
+      <c r="M26" s="15"/>
+      <c r="N26" s="15"/>
+      <c r="O26" s="15"/>
+      <c r="P26" s="15"/>
+      <c r="Q26" s="15"/>
+      <c r="R26" s="15"/>
+      <c r="S26" s="15"/>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -2236,7 +2472,7 @@
         <v>3E48</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -2296,7 +2532,7 @@
         <v>3155</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -2307,7 +2543,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -2367,7 +2603,7 @@
         <v>2044</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -2375,7 +2611,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -2437,7 +2673,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="33" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B33" t="s">
         <v>64</v>
       </c>
@@ -2445,8 +2681,1715 @@
         <v>66</v>
       </c>
     </row>
+    <row r="34" spans="2:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="B34" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34" s="7">
+        <v>1</v>
+      </c>
+      <c r="E34" s="7">
+        <v>0</v>
+      </c>
+      <c r="F34" s="7">
+        <v>0</v>
+      </c>
+      <c r="G34" s="7">
+        <v>1</v>
+      </c>
+      <c r="H34" s="7">
+        <v>0</v>
+      </c>
+      <c r="I34" s="7">
+        <v>0</v>
+      </c>
+      <c r="J34" s="7">
+        <v>1</v>
+      </c>
+      <c r="K34" s="7">
+        <v>0</v>
+      </c>
+      <c r="L34" s="7">
+        <v>0</v>
+      </c>
+      <c r="M34" s="7">
+        <v>0</v>
+      </c>
+      <c r="N34" s="7">
+        <v>0</v>
+      </c>
+      <c r="O34" s="7">
+        <v>0</v>
+      </c>
+      <c r="P34" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q34" s="7">
+        <v>0</v>
+      </c>
+      <c r="R34" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="C35" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14">
+        <v>9</v>
+      </c>
+      <c r="H35" s="14"/>
+      <c r="I35" s="14"/>
+      <c r="J35" s="14"/>
+      <c r="K35" s="14">
+        <v>0</v>
+      </c>
+      <c r="L35" s="14"/>
+      <c r="M35" s="14"/>
+      <c r="N35" s="14"/>
+      <c r="O35" s="14">
+        <v>0</v>
+      </c>
+      <c r="P35" s="14"/>
+      <c r="Q35" s="14"/>
+      <c r="R35" s="14"/>
+    </row>
+    <row r="36" spans="2:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="B36" t="s">
+        <v>50</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="G36" s="7">
+        <v>0</v>
+      </c>
+      <c r="H36" s="7">
+        <v>1</v>
+      </c>
+      <c r="I36" s="7">
+        <v>0</v>
+      </c>
+      <c r="J36" s="7">
+        <v>1</v>
+      </c>
+      <c r="K36" s="7">
+        <v>0</v>
+      </c>
+      <c r="L36" s="7">
+        <v>1</v>
+      </c>
+      <c r="M36" s="7">
+        <v>0</v>
+      </c>
+      <c r="N36" s="7">
+        <v>1</v>
+      </c>
+      <c r="O36" s="7">
+        <v>0</v>
+      </c>
+      <c r="P36" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q36" s="7">
+        <v>0</v>
+      </c>
+      <c r="R36" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="C37" s="14">
+        <v>1</v>
+      </c>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14">
+        <v>5</v>
+      </c>
+      <c r="H37" s="14"/>
+      <c r="I37" s="14"/>
+      <c r="J37" s="14"/>
+      <c r="K37" s="14">
+        <v>5</v>
+      </c>
+      <c r="L37" s="14"/>
+      <c r="M37" s="14"/>
+      <c r="N37" s="14"/>
+      <c r="O37" s="14">
+        <v>4</v>
+      </c>
+      <c r="P37" s="14"/>
+      <c r="Q37" s="14"/>
+      <c r="R37" s="14"/>
+    </row>
+    <row r="39" spans="2:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="B39" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="40" spans="2:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="B40" s="12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="41" spans="2:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="B41" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="42" spans="2:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="B42" t="s">
+        <v>109</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42">
+        <v>1</v>
+      </c>
+      <c r="G42">
+        <v>1</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42" s="4">
+        <v>1</v>
+      </c>
+      <c r="J42" s="4">
+        <v>1</v>
+      </c>
+      <c r="K42" s="4">
+        <v>0</v>
+      </c>
+      <c r="L42" s="4">
+        <v>1</v>
+      </c>
+      <c r="M42" s="4">
+        <v>1</v>
+      </c>
+      <c r="N42" s="4">
+        <v>0</v>
+      </c>
+      <c r="O42" s="4">
+        <v>1</v>
+      </c>
+      <c r="P42" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q42" s="4">
+        <v>0</v>
+      </c>
+      <c r="R42" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="2:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="I43" s="4"/>
+      <c r="J43" s="4"/>
+      <c r="K43" s="4"/>
+      <c r="L43" s="4"/>
+      <c r="M43" s="4"/>
+      <c r="N43" s="4"/>
+      <c r="O43" s="4"/>
+      <c r="P43" s="4"/>
+      <c r="Q43" s="4"/>
+      <c r="R43" s="4"/>
+    </row>
+    <row r="44" spans="2:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="B44" t="s">
+        <v>110</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>1</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+      <c r="H44">
+        <v>1</v>
+      </c>
+      <c r="I44" s="4">
+        <v>0</v>
+      </c>
+      <c r="J44" s="4">
+        <v>0</v>
+      </c>
+      <c r="K44" s="4">
+        <v>0</v>
+      </c>
+      <c r="L44" s="4">
+        <v>0</v>
+      </c>
+      <c r="M44" s="4">
+        <v>0</v>
+      </c>
+      <c r="N44" s="4">
+        <v>0</v>
+      </c>
+      <c r="O44" s="4">
+        <v>0</v>
+      </c>
+      <c r="P44" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q44" s="4">
+        <v>1</v>
+      </c>
+      <c r="R44" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="2:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="B46" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>1</v>
+      </c>
+      <c r="H46">
+        <v>1</v>
+      </c>
+      <c r="I46">
+        <v>0</v>
+      </c>
+      <c r="J46">
+        <v>1</v>
+      </c>
+      <c r="K46">
+        <v>0</v>
+      </c>
+      <c r="L46">
+        <v>0</v>
+      </c>
+      <c r="M46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="2:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <v>0</v>
+      </c>
+      <c r="J47">
+        <v>1</v>
+      </c>
+      <c r="K47">
+        <v>0</v>
+      </c>
+      <c r="L47">
+        <v>0</v>
+      </c>
+      <c r="M47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="2:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="B48" t="s">
+        <v>112</v>
+      </c>
+      <c r="C48" s="16">
+        <v>1</v>
+      </c>
+      <c r="D48" s="16">
+        <v>1</v>
+      </c>
+      <c r="E48" s="16">
+        <v>1</v>
+      </c>
+      <c r="F48" s="16">
+        <v>0</v>
+      </c>
+      <c r="G48" s="16">
+        <v>1</v>
+      </c>
+      <c r="H48" s="16">
+        <v>1</v>
+      </c>
+      <c r="I48" s="16">
+        <v>1</v>
+      </c>
+      <c r="J48" s="16">
+        <v>0</v>
+      </c>
+      <c r="K48" s="16">
+        <v>0</v>
+      </c>
+      <c r="L48" s="16">
+        <v>0</v>
+      </c>
+      <c r="M48" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B50" t="s">
+        <v>114</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50" s="4">
+        <v>0</v>
+      </c>
+      <c r="E50" s="4">
+        <v>1</v>
+      </c>
+      <c r="F50" s="4">
+        <v>1</v>
+      </c>
+      <c r="G50" s="4">
+        <v>1</v>
+      </c>
+      <c r="H50" s="4">
+        <v>0</v>
+      </c>
+      <c r="I50" s="16">
+        <v>1</v>
+      </c>
+      <c r="J50" s="16">
+        <v>1</v>
+      </c>
+      <c r="K50" s="16">
+        <v>0</v>
+      </c>
+      <c r="L50" s="16">
+        <v>1</v>
+      </c>
+      <c r="M50" s="16">
+        <v>1</v>
+      </c>
+      <c r="N50" s="16">
+        <v>1</v>
+      </c>
+      <c r="O50" s="16">
+        <v>0</v>
+      </c>
+      <c r="P50" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q50" s="16">
+        <v>0</v>
+      </c>
+      <c r="R50" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="C51" s="14">
+        <v>3</v>
+      </c>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14"/>
+      <c r="G51" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H51" s="14"/>
+      <c r="I51" s="14"/>
+      <c r="J51" s="14"/>
+      <c r="K51" s="14">
+        <v>7</v>
+      </c>
+      <c r="L51" s="14"/>
+      <c r="M51" s="14"/>
+      <c r="N51" s="14"/>
+      <c r="O51" s="14">
+        <v>1</v>
+      </c>
+      <c r="P51" s="14"/>
+      <c r="Q51" s="14"/>
+      <c r="R51" s="14"/>
+    </row>
+    <row r="53" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B53" t="s">
+        <v>119</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53" s="4">
+        <v>0</v>
+      </c>
+      <c r="E53" s="4">
+        <v>1</v>
+      </c>
+      <c r="F53" s="4">
+        <v>1</v>
+      </c>
+      <c r="G53" s="4">
+        <v>1</v>
+      </c>
+      <c r="H53" s="4">
+        <v>0</v>
+      </c>
+      <c r="I53">
+        <v>1</v>
+      </c>
+      <c r="J53">
+        <v>1</v>
+      </c>
+      <c r="K53">
+        <v>0</v>
+      </c>
+      <c r="L53">
+        <v>1</v>
+      </c>
+      <c r="M53">
+        <v>1</v>
+      </c>
+      <c r="N53">
+        <v>1</v>
+      </c>
+      <c r="O53">
+        <v>0</v>
+      </c>
+      <c r="P53">
+        <v>0</v>
+      </c>
+      <c r="Q53">
+        <v>1</v>
+      </c>
+      <c r="R53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B55" t="s">
+        <v>122</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55" s="4">
+        <v>0</v>
+      </c>
+      <c r="E55" s="4">
+        <v>1</v>
+      </c>
+      <c r="F55" s="4">
+        <v>0</v>
+      </c>
+      <c r="G55" s="4">
+        <v>1</v>
+      </c>
+      <c r="H55" s="4">
+        <v>0</v>
+      </c>
+      <c r="I55">
+        <v>0</v>
+      </c>
+      <c r="J55">
+        <v>1</v>
+      </c>
+      <c r="K55">
+        <v>0</v>
+      </c>
+      <c r="L55">
+        <v>1</v>
+      </c>
+      <c r="M55">
+        <v>1</v>
+      </c>
+      <c r="N55">
+        <v>1</v>
+      </c>
+      <c r="O55">
+        <v>1</v>
+      </c>
+      <c r="P55">
+        <v>1</v>
+      </c>
+      <c r="Q55">
+        <v>1</v>
+      </c>
+      <c r="R55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+      <c r="F57">
+        <v>0</v>
+      </c>
+      <c r="G57">
+        <v>1</v>
+      </c>
+      <c r="H57">
+        <v>1</v>
+      </c>
+      <c r="I57">
+        <v>1</v>
+      </c>
+      <c r="J57">
+        <v>0</v>
+      </c>
+      <c r="K57">
+        <v>0</v>
+      </c>
+      <c r="L57">
+        <v>1</v>
+      </c>
+      <c r="M57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58">
+        <v>0</v>
+      </c>
+      <c r="G58">
+        <v>1</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+      <c r="I58">
+        <v>1</v>
+      </c>
+      <c r="J58">
+        <v>0</v>
+      </c>
+      <c r="K58">
+        <v>1</v>
+      </c>
+      <c r="L58">
+        <v>1</v>
+      </c>
+      <c r="M58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="C59" s="17">
+        <v>1</v>
+      </c>
+      <c r="D59" s="17">
+        <v>1</v>
+      </c>
+      <c r="E59" s="17">
+        <v>1</v>
+      </c>
+      <c r="F59" s="17">
+        <v>1</v>
+      </c>
+      <c r="G59" s="17">
+        <v>1</v>
+      </c>
+      <c r="H59" s="17">
+        <v>0</v>
+      </c>
+      <c r="I59" s="17">
+        <v>0</v>
+      </c>
+      <c r="J59" s="17">
+        <v>1</v>
+      </c>
+      <c r="K59" s="17">
+        <v>0</v>
+      </c>
+      <c r="L59" s="17">
+        <v>1</v>
+      </c>
+      <c r="M59" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61">
+        <v>1</v>
+      </c>
+      <c r="F61">
+        <v>1</v>
+      </c>
+      <c r="G61">
+        <v>1</v>
+      </c>
+      <c r="H61">
+        <v>0</v>
+      </c>
+      <c r="I61" s="18">
+        <v>1</v>
+      </c>
+      <c r="J61" s="18">
+        <v>1</v>
+      </c>
+      <c r="K61" s="18">
+        <v>1</v>
+      </c>
+      <c r="L61" s="18">
+        <v>1</v>
+      </c>
+      <c r="M61" s="18">
+        <v>0</v>
+      </c>
+      <c r="N61" s="18">
+        <v>0</v>
+      </c>
+      <c r="O61" s="18">
+        <v>1</v>
+      </c>
+      <c r="P61" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q61" s="18">
+        <v>1</v>
+      </c>
+      <c r="R61" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="C62" s="14">
+        <v>3</v>
+      </c>
+      <c r="D62" s="14"/>
+      <c r="E62" s="14"/>
+      <c r="F62" s="14"/>
+      <c r="G62" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H62" s="14"/>
+      <c r="I62" s="14"/>
+      <c r="J62" s="14"/>
+      <c r="K62" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="L62" s="14"/>
+      <c r="M62" s="14"/>
+      <c r="N62" s="14"/>
+      <c r="O62" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="P62" s="14"/>
+      <c r="Q62" s="14"/>
+      <c r="R62" s="14"/>
+    </row>
+    <row r="64" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B64" t="s">
+        <v>127</v>
+      </c>
+      <c r="C64">
+        <v>1</v>
+      </c>
+      <c r="D64" s="7">
+        <v>1</v>
+      </c>
+      <c r="E64" s="7">
+        <v>0</v>
+      </c>
+      <c r="F64" s="7">
+        <v>0</v>
+      </c>
+      <c r="G64" s="7">
+        <v>1</v>
+      </c>
+      <c r="H64" s="7">
+        <v>0</v>
+      </c>
+      <c r="I64" s="7">
+        <v>0</v>
+      </c>
+      <c r="J64" s="7">
+        <v>1</v>
+      </c>
+      <c r="K64" s="7">
+        <v>0</v>
+      </c>
+      <c r="L64" s="7">
+        <v>0</v>
+      </c>
+      <c r="M64" s="7">
+        <v>0</v>
+      </c>
+      <c r="N64" s="7">
+        <v>0</v>
+      </c>
+      <c r="O64" s="7"/>
+    </row>
+    <row r="65" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B65" t="s">
+        <v>129</v>
+      </c>
+      <c r="C65" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="D65" s="14"/>
+      <c r="E65" s="14"/>
+      <c r="F65" s="14"/>
+      <c r="G65" s="14">
+        <v>9</v>
+      </c>
+      <c r="H65" s="14"/>
+      <c r="I65" s="14"/>
+      <c r="J65" s="14"/>
+      <c r="K65" s="14">
+        <v>0</v>
+      </c>
+      <c r="L65" s="14"/>
+      <c r="M65" s="14"/>
+      <c r="N65" s="14"/>
+    </row>
+    <row r="66" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B66" t="s">
+        <v>126</v>
+      </c>
+      <c r="C66" s="19">
+        <v>0</v>
+      </c>
+      <c r="D66" s="19">
+        <v>0</v>
+      </c>
+      <c r="E66" s="19">
+        <v>0</v>
+      </c>
+      <c r="F66" s="19">
+        <v>1</v>
+      </c>
+      <c r="G66" s="20">
+        <v>0</v>
+      </c>
+      <c r="H66" s="20">
+        <v>1</v>
+      </c>
+      <c r="I66" s="20">
+        <v>0</v>
+      </c>
+      <c r="J66" s="20">
+        <v>1</v>
+      </c>
+      <c r="K66" s="20">
+        <v>0</v>
+      </c>
+      <c r="L66" s="20">
+        <v>1</v>
+      </c>
+      <c r="M66" s="20">
+        <v>0</v>
+      </c>
+      <c r="N66" s="22">
+        <v>0</v>
+      </c>
+      <c r="O66" s="7"/>
+      <c r="P66" s="7"/>
+    </row>
+    <row r="67" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B67" t="s">
+        <v>129</v>
+      </c>
+      <c r="C67" s="21">
+        <v>1</v>
+      </c>
+      <c r="D67" s="21"/>
+      <c r="E67" s="21"/>
+      <c r="F67" s="21"/>
+      <c r="G67" s="21">
+        <v>5</v>
+      </c>
+      <c r="H67" s="21"/>
+      <c r="I67" s="21"/>
+      <c r="J67" s="21"/>
+      <c r="K67" s="14">
+        <v>4</v>
+      </c>
+      <c r="L67" s="14"/>
+      <c r="M67" s="14"/>
+      <c r="N67" s="14"/>
+    </row>
+    <row r="69" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="E69" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="70" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B70" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="71" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B71" t="s">
+        <v>132</v>
+      </c>
+      <c r="C71" s="6">
+        <v>0</v>
+      </c>
+      <c r="D71" s="7">
+        <v>0</v>
+      </c>
+      <c r="E71" s="7">
+        <v>1</v>
+      </c>
+      <c r="F71" s="7">
+        <v>1</v>
+      </c>
+      <c r="G71" s="7">
+        <v>1</v>
+      </c>
+      <c r="H71" s="7">
+        <v>1</v>
+      </c>
+      <c r="I71" s="7">
+        <v>1</v>
+      </c>
+      <c r="J71" s="7">
+        <v>0</v>
+      </c>
+      <c r="K71" s="7">
+        <v>0</v>
+      </c>
+      <c r="L71" s="7">
+        <v>1</v>
+      </c>
+      <c r="M71" s="7">
+        <v>0</v>
+      </c>
+      <c r="N71" s="7">
+        <v>0</v>
+      </c>
+      <c r="O71" s="7">
+        <v>1</v>
+      </c>
+      <c r="P71" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q71" s="7">
+        <v>0</v>
+      </c>
+      <c r="R71" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="C72" s="14"/>
+      <c r="D72" s="14"/>
+      <c r="E72" s="14"/>
+      <c r="F72" s="14"/>
+      <c r="G72" s="14"/>
+      <c r="H72" s="14"/>
+      <c r="I72" s="14"/>
+      <c r="J72" s="14"/>
+      <c r="K72" s="14"/>
+      <c r="L72" s="14"/>
+      <c r="M72" s="14"/>
+      <c r="N72" s="14"/>
+      <c r="O72" s="14"/>
+      <c r="P72" s="14"/>
+      <c r="Q72" s="14"/>
+      <c r="R72" s="14"/>
+    </row>
+    <row r="73" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B73" t="s">
+        <v>116</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="E73">
+        <v>1</v>
+      </c>
+      <c r="F73">
+        <v>1</v>
+      </c>
+      <c r="G73">
+        <v>0</v>
+      </c>
+      <c r="H73">
+        <v>1</v>
+      </c>
+      <c r="I73">
+        <v>0</v>
+      </c>
+      <c r="J73">
+        <v>0</v>
+      </c>
+      <c r="K73">
+        <v>0</v>
+      </c>
+      <c r="L73">
+        <v>0</v>
+      </c>
+      <c r="M73">
+        <v>1</v>
+      </c>
+      <c r="N73">
+        <v>0</v>
+      </c>
+      <c r="O73">
+        <v>1</v>
+      </c>
+      <c r="P73">
+        <v>0</v>
+      </c>
+      <c r="Q73">
+        <v>1</v>
+      </c>
+      <c r="R73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B75" t="s">
+        <v>128</v>
+      </c>
+      <c r="C75">
+        <v>1</v>
+      </c>
+      <c r="D75" s="7">
+        <v>1</v>
+      </c>
+      <c r="E75" s="7">
+        <v>0</v>
+      </c>
+      <c r="F75" s="7">
+        <v>0</v>
+      </c>
+      <c r="G75" s="7">
+        <v>1</v>
+      </c>
+      <c r="H75" s="7">
+        <v>0</v>
+      </c>
+      <c r="I75" s="7">
+        <v>0</v>
+      </c>
+      <c r="J75" s="7">
+        <v>1</v>
+      </c>
+      <c r="K75" s="7">
+        <v>0</v>
+      </c>
+      <c r="L75" s="7">
+        <v>0</v>
+      </c>
+      <c r="M75" s="7">
+        <v>0</v>
+      </c>
+      <c r="N75" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="C76" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="D76" s="14"/>
+      <c r="E76" s="14"/>
+      <c r="F76" s="14"/>
+      <c r="G76" s="14">
+        <v>9</v>
+      </c>
+      <c r="H76" s="14"/>
+      <c r="I76" s="14"/>
+      <c r="J76" s="14"/>
+      <c r="K76" s="14">
+        <v>0</v>
+      </c>
+      <c r="L76" s="14"/>
+      <c r="M76" s="14"/>
+      <c r="N76" s="14"/>
+    </row>
+    <row r="77" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B77" t="s">
+        <v>131</v>
+      </c>
+      <c r="C77">
+        <v>0</v>
+      </c>
+      <c r="D77">
+        <v>0</v>
+      </c>
+      <c r="E77">
+        <v>1</v>
+      </c>
+      <c r="F77">
+        <v>0</v>
+      </c>
+      <c r="G77">
+        <v>0</v>
+      </c>
+      <c r="H77">
+        <v>0</v>
+      </c>
+      <c r="I77">
+        <v>0</v>
+      </c>
+      <c r="J77">
+        <v>1</v>
+      </c>
+      <c r="K77">
+        <v>0</v>
+      </c>
+      <c r="L77">
+        <v>1</v>
+      </c>
+      <c r="M77">
+        <v>0</v>
+      </c>
+      <c r="N77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="C78" s="14">
+        <v>2</v>
+      </c>
+      <c r="D78" s="14"/>
+      <c r="E78" s="14"/>
+      <c r="F78" s="14"/>
+      <c r="G78" s="14">
+        <v>1</v>
+      </c>
+      <c r="H78" s="14"/>
+      <c r="I78" s="14"/>
+      <c r="J78" s="14"/>
+      <c r="K78" s="14">
+        <v>4</v>
+      </c>
+      <c r="L78" s="14"/>
+      <c r="M78" s="14"/>
+      <c r="N78" s="14"/>
+    </row>
+    <row r="80" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="C80" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="81" spans="2:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="C81" s="14">
+        <v>1</v>
+      </c>
+      <c r="D81" s="14"/>
+      <c r="E81" s="14"/>
+      <c r="F81" s="14"/>
+      <c r="G81" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="H81" s="14"/>
+      <c r="I81" s="14"/>
+      <c r="J81" s="14"/>
+      <c r="K81" s="14">
+        <v>1</v>
+      </c>
+      <c r="L81" s="14"/>
+      <c r="M81" s="14"/>
+      <c r="N81" s="14"/>
+      <c r="O81" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="P81" s="14"/>
+      <c r="Q81" s="14"/>
+      <c r="R81" s="14"/>
+      <c r="S81" s="14">
+        <v>4</v>
+      </c>
+      <c r="T81" s="14"/>
+      <c r="U81" s="14"/>
+      <c r="V81" s="14"/>
+    </row>
+    <row r="82" spans="2:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="C82">
+        <v>0</v>
+      </c>
+      <c r="D82">
+        <v>0</v>
+      </c>
+      <c r="E82">
+        <v>0</v>
+      </c>
+      <c r="F82">
+        <v>1</v>
+      </c>
+      <c r="G82">
+        <v>1</v>
+      </c>
+      <c r="H82">
+        <v>0</v>
+      </c>
+      <c r="I82">
+        <v>1</v>
+      </c>
+      <c r="J82">
+        <v>0</v>
+      </c>
+      <c r="K82">
+        <v>0</v>
+      </c>
+      <c r="L82">
+        <v>0</v>
+      </c>
+      <c r="M82">
+        <v>0</v>
+      </c>
+      <c r="N82">
+        <v>1</v>
+      </c>
+      <c r="O82">
+        <v>1</v>
+      </c>
+      <c r="P82">
+        <v>0</v>
+      </c>
+      <c r="Q82">
+        <v>1</v>
+      </c>
+      <c r="R82">
+        <v>1</v>
+      </c>
+      <c r="S82">
+        <v>0</v>
+      </c>
+      <c r="T82">
+        <v>1</v>
+      </c>
+      <c r="U82">
+        <v>0</v>
+      </c>
+      <c r="V82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="2:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="C84" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="D84" s="14"/>
+      <c r="E84" s="14"/>
+      <c r="F84" s="14"/>
+      <c r="G84" s="14"/>
+      <c r="H84" s="14"/>
+      <c r="I84" s="14"/>
+      <c r="J84" s="14"/>
+      <c r="K84" s="14"/>
+      <c r="L84" s="14"/>
+    </row>
+    <row r="85" spans="2:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="C85">
+        <v>1</v>
+      </c>
+      <c r="D85">
+        <v>0</v>
+      </c>
+      <c r="E85">
+        <v>1</v>
+      </c>
+      <c r="F85">
+        <v>0</v>
+      </c>
+      <c r="G85">
+        <v>0</v>
+      </c>
+      <c r="H85">
+        <v>0</v>
+      </c>
+      <c r="I85">
+        <v>0</v>
+      </c>
+      <c r="J85">
+        <v>1</v>
+      </c>
+      <c r="K85">
+        <v>1</v>
+      </c>
+      <c r="L85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="2:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="C86" s="7"/>
+      <c r="D86" s="7"/>
+      <c r="E86" s="14">
+        <v>8</v>
+      </c>
+      <c r="F86" s="14"/>
+      <c r="G86" s="14"/>
+      <c r="H86" s="14"/>
+      <c r="I86" s="14">
+        <v>6</v>
+      </c>
+      <c r="J86" s="14"/>
+      <c r="K86" s="14"/>
+      <c r="L86" s="14"/>
+    </row>
+    <row r="87" spans="2:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="B87" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="89" spans="2:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="B89" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="90" spans="2:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="B90" t="s">
+        <v>119</v>
+      </c>
+      <c r="C90">
+        <v>0</v>
+      </c>
+      <c r="D90">
+        <v>0</v>
+      </c>
+      <c r="E90">
+        <v>1</v>
+      </c>
+      <c r="F90">
+        <v>1</v>
+      </c>
+      <c r="G90">
+        <v>1</v>
+      </c>
+      <c r="H90">
+        <v>0</v>
+      </c>
+      <c r="I90">
+        <v>1</v>
+      </c>
+      <c r="J90">
+        <v>1</v>
+      </c>
+      <c r="K90">
+        <v>0</v>
+      </c>
+      <c r="L90">
+        <v>1</v>
+      </c>
+      <c r="M90">
+        <v>1</v>
+      </c>
+      <c r="N90">
+        <v>1</v>
+      </c>
+      <c r="O90">
+        <v>0</v>
+      </c>
+      <c r="P90">
+        <v>0</v>
+      </c>
+      <c r="Q90">
+        <v>1</v>
+      </c>
+      <c r="R90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="2:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="B92" t="s">
+        <v>123</v>
+      </c>
+      <c r="C92">
+        <v>0</v>
+      </c>
+      <c r="D92">
+        <v>0</v>
+      </c>
+      <c r="E92">
+        <v>1</v>
+      </c>
+      <c r="F92">
+        <v>0</v>
+      </c>
+      <c r="G92">
+        <v>1</v>
+      </c>
+      <c r="H92">
+        <v>1</v>
+      </c>
+      <c r="I92">
+        <v>0</v>
+      </c>
+      <c r="J92">
+        <v>0</v>
+      </c>
+      <c r="K92">
+        <v>0</v>
+      </c>
+      <c r="L92">
+        <v>0</v>
+      </c>
+      <c r="M92">
+        <v>1</v>
+      </c>
+      <c r="N92">
+        <v>1</v>
+      </c>
+      <c r="O92">
+        <v>1</v>
+      </c>
+      <c r="P92">
+        <v>0</v>
+      </c>
+      <c r="Q92">
+        <v>0</v>
+      </c>
+      <c r="R92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="2:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="C94">
+        <v>1</v>
+      </c>
+      <c r="D94">
+        <v>1</v>
+      </c>
+      <c r="E94">
+        <v>1</v>
+      </c>
+      <c r="F94">
+        <v>0</v>
+      </c>
+      <c r="G94">
+        <v>1</v>
+      </c>
+      <c r="H94">
+        <v>1</v>
+      </c>
+      <c r="I94">
+        <v>1</v>
+      </c>
+      <c r="J94">
+        <v>0</v>
+      </c>
+      <c r="K94">
+        <v>0</v>
+      </c>
+      <c r="L94">
+        <v>1</v>
+      </c>
+      <c r="M94">
+        <v>1</v>
+      </c>
+      <c r="N94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="2:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="C95" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="D95" s="14"/>
+      <c r="E95" s="14"/>
+      <c r="F95" s="14"/>
+      <c r="G95" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="H95" s="14"/>
+      <c r="I95" s="14"/>
+      <c r="J95" s="14"/>
+      <c r="K95" s="14">
+        <v>6</v>
+      </c>
+      <c r="L95" s="14"/>
+      <c r="M95" s="14"/>
+      <c r="N95" s="14"/>
+    </row>
+    <row r="96" spans="2:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="C96">
+        <v>0</v>
+      </c>
+      <c r="D96">
+        <v>0</v>
+      </c>
+      <c r="E96">
+        <v>0</v>
+      </c>
+      <c r="F96">
+        <v>1</v>
+      </c>
+      <c r="G96">
+        <v>0</v>
+      </c>
+      <c r="H96">
+        <v>0</v>
+      </c>
+      <c r="I96">
+        <v>0</v>
+      </c>
+      <c r="J96">
+        <v>0</v>
+      </c>
+      <c r="K96">
+        <v>1</v>
+      </c>
+      <c r="L96">
+        <v>1</v>
+      </c>
+      <c r="M96">
+        <v>1</v>
+      </c>
+      <c r="N96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="C97" s="14">
+        <v>1</v>
+      </c>
+      <c r="D97" s="14"/>
+      <c r="E97" s="14"/>
+      <c r="F97" s="14"/>
+      <c r="G97" s="14">
+        <v>0</v>
+      </c>
+      <c r="H97" s="14"/>
+      <c r="I97" s="14"/>
+      <c r="J97" s="14"/>
+      <c r="K97" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="L97" s="14"/>
+      <c r="M97" s="14"/>
+      <c r="N97" s="14"/>
+    </row>
+    <row r="98" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B98" t="s">
+        <v>112</v>
+      </c>
+      <c r="C98">
+        <v>1</v>
+      </c>
+      <c r="D98">
+        <v>1</v>
+      </c>
+      <c r="E98">
+        <v>1</v>
+      </c>
+      <c r="F98">
+        <v>1</v>
+      </c>
+      <c r="G98">
+        <v>1</v>
+      </c>
+      <c r="H98">
+        <v>1</v>
+      </c>
+      <c r="I98">
+        <v>1</v>
+      </c>
+      <c r="J98">
+        <v>1</v>
+      </c>
+      <c r="K98">
+        <v>0</v>
+      </c>
+      <c r="L98">
+        <v>1</v>
+      </c>
+      <c r="M98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B100" t="s">
+        <v>138</v>
+      </c>
+      <c r="C100">
+        <v>0</v>
+      </c>
+      <c r="D100">
+        <v>0</v>
+      </c>
+      <c r="E100">
+        <v>1</v>
+      </c>
+      <c r="F100">
+        <v>1</v>
+      </c>
+      <c r="G100">
+        <v>1</v>
+      </c>
+      <c r="H100">
+        <v>0</v>
+      </c>
+      <c r="I100">
+        <v>1</v>
+      </c>
+      <c r="J100">
+        <v>1</v>
+      </c>
+      <c r="K100">
+        <v>1</v>
+      </c>
+      <c r="L100">
+        <v>1</v>
+      </c>
+      <c r="M100">
+        <v>1</v>
+      </c>
+      <c r="N100">
+        <v>1</v>
+      </c>
+      <c r="O100">
+        <v>1</v>
+      </c>
+      <c r="P100">
+        <v>0</v>
+      </c>
+      <c r="Q100">
+        <v>1</v>
+      </c>
+      <c r="R100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="C101" s="14">
+        <v>3</v>
+      </c>
+      <c r="D101" s="14"/>
+      <c r="E101" s="14"/>
+      <c r="F101" s="14"/>
+      <c r="G101" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H101" s="14"/>
+      <c r="I101" s="14"/>
+      <c r="J101" s="14"/>
+      <c r="K101" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="L101" s="14"/>
+      <c r="M101" s="14"/>
+      <c r="N101" s="14"/>
+      <c r="O101" s="14">
+        <v>5</v>
+      </c>
+      <c r="P101" s="14"/>
+      <c r="Q101" s="14"/>
+      <c r="R101" s="14"/>
+    </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="74">
+    <mergeCell ref="C101:F101"/>
+    <mergeCell ref="G101:J101"/>
+    <mergeCell ref="K101:N101"/>
+    <mergeCell ref="O101:R101"/>
+    <mergeCell ref="C95:F95"/>
+    <mergeCell ref="G95:J95"/>
+    <mergeCell ref="K95:N95"/>
+    <mergeCell ref="C97:F97"/>
+    <mergeCell ref="G97:J97"/>
+    <mergeCell ref="K97:N97"/>
+    <mergeCell ref="O81:R81"/>
+    <mergeCell ref="S81:V81"/>
+    <mergeCell ref="I86:L86"/>
+    <mergeCell ref="C84:L84"/>
+    <mergeCell ref="E86:H86"/>
+    <mergeCell ref="C78:F78"/>
+    <mergeCell ref="G78:J78"/>
+    <mergeCell ref="K78:N78"/>
+    <mergeCell ref="C81:F81"/>
+    <mergeCell ref="G81:J81"/>
+    <mergeCell ref="K81:N81"/>
+    <mergeCell ref="C72:F72"/>
+    <mergeCell ref="G72:J72"/>
+    <mergeCell ref="K72:N72"/>
+    <mergeCell ref="O72:R72"/>
+    <mergeCell ref="C76:F76"/>
+    <mergeCell ref="G76:J76"/>
+    <mergeCell ref="K76:N76"/>
+    <mergeCell ref="C65:F65"/>
+    <mergeCell ref="G65:J65"/>
+    <mergeCell ref="K65:N65"/>
+    <mergeCell ref="C67:F67"/>
+    <mergeCell ref="G67:J67"/>
+    <mergeCell ref="K67:N67"/>
+    <mergeCell ref="C51:F51"/>
+    <mergeCell ref="G51:J51"/>
+    <mergeCell ref="K51:N51"/>
+    <mergeCell ref="O51:R51"/>
+    <mergeCell ref="C62:F62"/>
+    <mergeCell ref="G62:J62"/>
+    <mergeCell ref="K62:N62"/>
+    <mergeCell ref="O62:R62"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="M4:P4"/>
     <mergeCell ref="I6:J6"/>
@@ -2471,6 +4414,14 @@
     <mergeCell ref="K3:N3"/>
     <mergeCell ref="O3:P3"/>
     <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="O35:R35"/>
+    <mergeCell ref="C37:F37"/>
+    <mergeCell ref="G37:J37"/>
+    <mergeCell ref="K37:N37"/>
+    <mergeCell ref="O37:R37"/>
+    <mergeCell ref="C35:F35"/>
+    <mergeCell ref="G35:J35"/>
+    <mergeCell ref="K35:N35"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2483,65 +4434,65 @@
   <dimension ref="A1:AH19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="19.6640625" customWidth="1"/>
-    <col min="3" max="3" width="12.5546875" customWidth="1"/>
-    <col min="4" max="36" width="4.6640625" customWidth="1"/>
-    <col min="37" max="37" width="4.33203125" customWidth="1"/>
+    <col min="2" max="2" width="19.68359375" customWidth="1"/>
+    <col min="3" max="3" width="12.5234375" customWidth="1"/>
+    <col min="4" max="36" width="4.68359375" customWidth="1"/>
+    <col min="37" max="37" width="4.3125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13"/>
-      <c r="W1" s="13"/>
-      <c r="X1" s="13"/>
-      <c r="Y1" s="13"/>
-      <c r="Z1" s="13"/>
-      <c r="AA1" s="13"/>
-      <c r="AB1" s="13"/>
-      <c r="AC1" s="13"/>
-      <c r="AD1" s="13"/>
-      <c r="AE1" s="13"/>
-      <c r="AF1" s="13"/>
-      <c r="AG1" s="13"/>
-      <c r="AH1" s="13"/>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
+      <c r="W1" s="15"/>
+      <c r="X1" s="15"/>
+      <c r="Y1" s="15"/>
+      <c r="Z1" s="15"/>
+      <c r="AA1" s="15"/>
+      <c r="AB1" s="15"/>
+      <c r="AC1" s="15"/>
+      <c r="AD1" s="15"/>
+      <c r="AE1" s="15"/>
+      <c r="AF1" s="15"/>
+      <c r="AG1" s="15"/>
+      <c r="AH1" s="15"/>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
       <c r="D2">
         <v>0</v>
       </c>
@@ -2636,7 +4587,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -2658,7 +4609,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -2680,7 +4631,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -2705,7 +4656,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -2730,7 +4681,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -2755,7 +4706,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -2780,7 +4731,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -2802,7 +4753,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -2827,7 +4778,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -2852,7 +4803,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -2877,7 +4828,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -2902,7 +4853,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -2927,7 +4878,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -2952,7 +4903,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -2977,7 +4928,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>45</v>
       </c>
@@ -2999,7 +4950,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>46</v>
       </c>
@@ -3024,7 +4975,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
fix(fpu): fix the addition of half precission numbers #2
</commit_message>
<xml_diff>
--- a/programs/pipelining/fpumaclaurinprogramsinpiover2.xlsx
+++ b/programs/pipelining/fpumaclaurinprogramsinpiover2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vacla\Projects\cpu\programs\pipelining\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66803C3B-1AF0-4420-90AA-4AD4E8C79974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA4C1615-983B-4A60-8AA0-C82B09F7C9EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{E410B2C1-F054-41C4-A96D-F1120FBD95E0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E410B2C1-F054-41C4-A96D-F1120FBD95E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Code" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="140">
   <si>
     <t>Hex</t>
   </si>
@@ -409,9 +409,6 @@
     <t>0x2c38</t>
   </si>
   <si>
-    <t>0x2ffa</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -455,6 +452,9 @@
   </si>
   <si>
     <t>e</t>
+  </si>
+  <si>
+    <t>0x3BFA</t>
   </si>
 </sst>
 </file>
@@ -551,21 +551,21 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -881,24 +881,24 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8E17FB6-AC76-4C3E-BEFA-6AB3607784FD}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Y101"/>
+  <dimension ref="A1:Z103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D96" sqref="D96"/>
+    <sheetView tabSelected="1" topLeftCell="O7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Z23" sqref="Z23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.3125" customWidth="1"/>
-    <col min="2" max="2" width="22.7890625" customWidth="1"/>
-    <col min="20" max="20" width="22.89453125" customWidth="1"/>
-    <col min="21" max="21" width="19.68359375" customWidth="1"/>
-    <col min="22" max="22" width="18.5234375" customWidth="1"/>
-    <col min="23" max="23" width="30.3125" customWidth="1"/>
-    <col min="24" max="24" width="27.89453125" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" customWidth="1"/>
+    <col min="2" max="2" width="22.77734375" customWidth="1"/>
+    <col min="20" max="20" width="22.88671875" customWidth="1"/>
+    <col min="21" max="21" width="19.6640625" customWidth="1"/>
+    <col min="22" max="22" width="18.5546875" customWidth="1"/>
+    <col min="23" max="23" width="30.33203125" customWidth="1"/>
+    <col min="24" max="24" width="27.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
       <c r="C1">
         <v>15</v>
       </c>
@@ -948,79 +948,79 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15" t="s">
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="15"/>
+      <c r="H2" s="22"/>
       <c r="I2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="15" t="s">
+      <c r="K2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15" t="s">
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="15"/>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="22"/>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15" t="s">
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="15"/>
+      <c r="H3" s="22"/>
       <c r="I3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="15" t="s">
+      <c r="K3" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15"/>
-      <c r="O3" s="15" t="s">
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="P3" s="15"/>
-      <c r="Q3" s="15" t="s">
+      <c r="P3" s="22"/>
+      <c r="Q3" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="R3" s="15"/>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="R3" s="22"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>13</v>
       </c>
@@ -1036,10 +1036,10 @@
       <c r="F4" s="1">
         <v>0</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="G4" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="15"/>
+      <c r="H4" s="22"/>
       <c r="I4" s="1" t="s">
         <v>14</v>
       </c>
@@ -1052,93 +1052,93 @@
       <c r="L4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="15" t="s">
+      <c r="M4" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="N4" s="15"/>
-      <c r="O4" s="15"/>
-      <c r="P4" s="15"/>
-      <c r="Q4" s="15" t="s">
+      <c r="N4" s="22"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="22"/>
+      <c r="Q4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="R4" s="15"/>
-    </row>
-    <row r="5" spans="1:25" ht="11.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="R4" s="22"/>
+    </row>
+    <row r="5" spans="1:25" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15" t="s">
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
-      <c r="P5" s="15"/>
-      <c r="Q5" s="15"/>
-      <c r="R5" s="15"/>
-    </row>
-    <row r="6" spans="1:25" ht="13.2" hidden="1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="22"/>
+      <c r="M5" s="22"/>
+      <c r="N5" s="22"/>
+      <c r="O5" s="22"/>
+      <c r="P5" s="22"/>
+      <c r="Q5" s="22"/>
+      <c r="R5" s="22"/>
+    </row>
+    <row r="6" spans="1:25" ht="13.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15" t="s">
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15" t="s">
+      <c r="H6" s="22"/>
+      <c r="I6" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15" t="s">
+      <c r="J6" s="22"/>
+      <c r="K6" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="15" t="s">
+      <c r="L6" s="22"/>
+      <c r="M6" s="22"/>
+      <c r="N6" s="22"/>
+      <c r="O6" s="22"/>
+      <c r="P6" s="22"/>
+      <c r="Q6" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="R6" s="15"/>
-    </row>
-    <row r="7" spans="1:25" ht="63.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="R6" s="22"/>
+    </row>
+    <row r="7" spans="1:25" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15" t="s">
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15" t="s">
+      <c r="H7" s="22"/>
+      <c r="I7" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="J7" s="15"/>
+      <c r="J7" s="22"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
@@ -1169,36 +1169,36 @@
         <v>115</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="13.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="15" t="s">
+    <row r="8" spans="1:25" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="15"/>
-      <c r="P8" s="15"/>
-      <c r="Q8" s="15"/>
-      <c r="R8" s="15"/>
-      <c r="S8" s="15"/>
-      <c r="T8" s="15"/>
-      <c r="U8" s="15"/>
-      <c r="V8" s="15"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="22"/>
+      <c r="O8" s="22"/>
+      <c r="P8" s="22"/>
+      <c r="Q8" s="22"/>
+      <c r="R8" s="22"/>
+      <c r="S8" s="22"/>
+      <c r="T8" s="22"/>
+      <c r="U8" s="22"/>
+      <c r="V8" s="22"/>
       <c r="W8" s="11"/>
       <c r="X8" s="8"/>
       <c r="Y8" s="8"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -1264,7 +1264,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1333,7 +1333,7 @@
         <v>1.5703125</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1402,7 +1402,7 @@
         <v>0.1666259765625</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -1477,7 +1477,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -1552,7 +1552,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -1627,7 +1627,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -1702,7 +1702,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1762,7 +1762,7 @@
         <v>D44</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -1834,7 +1834,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -1906,7 +1906,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>41</v>
       </c>
@@ -1978,7 +1978,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>42</v>
       </c>
@@ -2050,7 +2050,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -2122,7 +2122,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>44</v>
       </c>
@@ -2194,7 +2194,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>45</v>
       </c>
@@ -2266,10 +2266,13 @@
         <v>108</v>
       </c>
       <c r="Y23" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+        <v>139</v>
+      </c>
+      <c r="Z23">
+        <v>0.997</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -2329,7 +2332,7 @@
         <v>D44</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -2389,30 +2392,30 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="15" t="s">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A26" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="15"/>
-      <c r="I26" s="15"/>
-      <c r="J26" s="15"/>
-      <c r="K26" s="15"/>
-      <c r="L26" s="15"/>
-      <c r="M26" s="15"/>
-      <c r="N26" s="15"/>
-      <c r="O26" s="15"/>
-      <c r="P26" s="15"/>
-      <c r="Q26" s="15"/>
-      <c r="R26" s="15"/>
-      <c r="S26" s="15"/>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="22"/>
+      <c r="J26" s="22"/>
+      <c r="K26" s="22"/>
+      <c r="L26" s="22"/>
+      <c r="M26" s="22"/>
+      <c r="N26" s="22"/>
+      <c r="O26" s="22"/>
+      <c r="P26" s="22"/>
+      <c r="Q26" s="22"/>
+      <c r="R26" s="22"/>
+      <c r="S26" s="22"/>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -2472,7 +2475,7 @@
         <v>3E48</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -2532,7 +2535,7 @@
         <v>3155</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -2543,7 +2546,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -2603,7 +2606,7 @@
         <v>2044</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -2611,7 +2614,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -2673,7 +2676,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="33" spans="2:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>64</v>
       </c>
@@ -2681,7 +2684,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="2:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>49</v>
       </c>
@@ -2734,33 +2737,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:20" x14ac:dyDescent="0.55000000000000004">
-      <c r="C35" s="14" t="s">
+    <row r="35" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="C35" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14">
+      <c r="D35" s="20"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="20">
         <v>9</v>
       </c>
-      <c r="H35" s="14"/>
-      <c r="I35" s="14"/>
-      <c r="J35" s="14"/>
-      <c r="K35" s="14">
-        <v>0</v>
-      </c>
-      <c r="L35" s="14"/>
-      <c r="M35" s="14"/>
-      <c r="N35" s="14"/>
-      <c r="O35" s="14">
-        <v>0</v>
-      </c>
-      <c r="P35" s="14"/>
-      <c r="Q35" s="14"/>
-      <c r="R35" s="14"/>
-    </row>
-    <row r="36" spans="2:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="H35" s="20"/>
+      <c r="I35" s="20"/>
+      <c r="J35" s="20"/>
+      <c r="K35" s="20">
+        <v>0</v>
+      </c>
+      <c r="L35" s="20"/>
+      <c r="M35" s="20"/>
+      <c r="N35" s="20"/>
+      <c r="O35" s="20">
+        <v>0</v>
+      </c>
+      <c r="P35" s="20"/>
+      <c r="Q35" s="20"/>
+      <c r="R35" s="20"/>
+    </row>
+    <row r="36" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>50</v>
       </c>
@@ -2813,48 +2816,48 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:20" x14ac:dyDescent="0.55000000000000004">
-      <c r="C37" s="14">
-        <v>1</v>
-      </c>
-      <c r="D37" s="14"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14">
+    <row r="37" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="C37" s="20">
+        <v>1</v>
+      </c>
+      <c r="D37" s="20"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="20">
         <v>5</v>
       </c>
-      <c r="H37" s="14"/>
-      <c r="I37" s="14"/>
-      <c r="J37" s="14"/>
-      <c r="K37" s="14">
+      <c r="H37" s="20"/>
+      <c r="I37" s="20"/>
+      <c r="J37" s="20"/>
+      <c r="K37" s="20">
         <v>5</v>
       </c>
-      <c r="L37" s="14"/>
-      <c r="M37" s="14"/>
-      <c r="N37" s="14"/>
-      <c r="O37" s="14">
+      <c r="L37" s="20"/>
+      <c r="M37" s="20"/>
+      <c r="N37" s="20"/>
+      <c r="O37" s="20">
         <v>4</v>
       </c>
-      <c r="P37" s="14"/>
-      <c r="Q37" s="14"/>
-      <c r="R37" s="14"/>
-    </row>
-    <row r="39" spans="2:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="P37" s="20"/>
+      <c r="Q37" s="20"/>
+      <c r="R37" s="20"/>
+    </row>
+    <row r="39" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="40" spans="2:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B40" s="12" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="41" spans="2:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="42" spans="2:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>109</v>
       </c>
@@ -2907,7 +2910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="2:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="2:20" x14ac:dyDescent="0.3">
       <c r="I43" s="4"/>
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
@@ -2919,7 +2922,7 @@
       <c r="Q43" s="4"/>
       <c r="R43" s="4"/>
     </row>
-    <row r="44" spans="2:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>110</v>
       </c>
@@ -2972,7 +2975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B46" s="13" t="s">
         <v>113</v>
       </c>
@@ -3010,7 +3013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="2:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="2:20" x14ac:dyDescent="0.3">
       <c r="C47">
         <v>0</v>
       </c>
@@ -3045,45 +3048,45 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>112</v>
       </c>
-      <c r="C48" s="16">
-        <v>1</v>
-      </c>
-      <c r="D48" s="16">
-        <v>1</v>
-      </c>
-      <c r="E48" s="16">
-        <v>1</v>
-      </c>
-      <c r="F48" s="16">
-        <v>0</v>
-      </c>
-      <c r="G48" s="16">
-        <v>1</v>
-      </c>
-      <c r="H48" s="16">
-        <v>1</v>
-      </c>
-      <c r="I48" s="16">
-        <v>1</v>
-      </c>
-      <c r="J48" s="16">
-        <v>0</v>
-      </c>
-      <c r="K48" s="16">
-        <v>0</v>
-      </c>
-      <c r="L48" s="16">
-        <v>0</v>
-      </c>
-      <c r="M48" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="C48" s="14">
+        <v>1</v>
+      </c>
+      <c r="D48" s="14">
+        <v>1</v>
+      </c>
+      <c r="E48" s="14">
+        <v>1</v>
+      </c>
+      <c r="F48" s="14">
+        <v>0</v>
+      </c>
+      <c r="G48" s="14">
+        <v>1</v>
+      </c>
+      <c r="H48" s="14">
+        <v>1</v>
+      </c>
+      <c r="I48" s="14">
+        <v>1</v>
+      </c>
+      <c r="J48" s="14">
+        <v>0</v>
+      </c>
+      <c r="K48" s="14">
+        <v>0</v>
+      </c>
+      <c r="L48" s="14">
+        <v>0</v>
+      </c>
+      <c r="M48" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>114</v>
       </c>
@@ -3105,64 +3108,64 @@
       <c r="H50" s="4">
         <v>0</v>
       </c>
-      <c r="I50" s="16">
-        <v>1</v>
-      </c>
-      <c r="J50" s="16">
-        <v>1</v>
-      </c>
-      <c r="K50" s="16">
-        <v>0</v>
-      </c>
-      <c r="L50" s="16">
-        <v>1</v>
-      </c>
-      <c r="M50" s="16">
-        <v>1</v>
-      </c>
-      <c r="N50" s="16">
-        <v>1</v>
-      </c>
-      <c r="O50" s="16">
-        <v>0</v>
-      </c>
-      <c r="P50" s="16">
-        <v>0</v>
-      </c>
-      <c r="Q50" s="16">
-        <v>0</v>
-      </c>
-      <c r="R50" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="C51" s="14">
+      <c r="I50" s="14">
+        <v>1</v>
+      </c>
+      <c r="J50" s="14">
+        <v>1</v>
+      </c>
+      <c r="K50" s="14">
+        <v>0</v>
+      </c>
+      <c r="L50" s="14">
+        <v>1</v>
+      </c>
+      <c r="M50" s="14">
+        <v>1</v>
+      </c>
+      <c r="N50" s="14">
+        <v>1</v>
+      </c>
+      <c r="O50" s="14">
+        <v>0</v>
+      </c>
+      <c r="P50" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q50" s="14">
+        <v>0</v>
+      </c>
+      <c r="R50" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="C51" s="20">
         <v>3</v>
       </c>
-      <c r="D51" s="14"/>
-      <c r="E51" s="14"/>
-      <c r="F51" s="14"/>
-      <c r="G51" s="14" t="s">
+      <c r="D51" s="20"/>
+      <c r="E51" s="20"/>
+      <c r="F51" s="20"/>
+      <c r="G51" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="H51" s="14"/>
-      <c r="I51" s="14"/>
-      <c r="J51" s="14"/>
-      <c r="K51" s="14">
+      <c r="H51" s="20"/>
+      <c r="I51" s="20"/>
+      <c r="J51" s="20"/>
+      <c r="K51" s="20">
         <v>7</v>
       </c>
-      <c r="L51" s="14"/>
-      <c r="M51" s="14"/>
-      <c r="N51" s="14"/>
-      <c r="O51" s="14">
-        <v>1</v>
-      </c>
-      <c r="P51" s="14"/>
-      <c r="Q51" s="14"/>
-      <c r="R51" s="14"/>
-    </row>
-    <row r="53" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="L51" s="20"/>
+      <c r="M51" s="20"/>
+      <c r="N51" s="20"/>
+      <c r="O51" s="20">
+        <v>1</v>
+      </c>
+      <c r="P51" s="20"/>
+      <c r="Q51" s="20"/>
+      <c r="R51" s="20"/>
+    </row>
+    <row r="53" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>119</v>
       </c>
@@ -3215,7 +3218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>122</v>
       </c>
@@ -3268,7 +3271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C57">
         <v>1</v>
       </c>
@@ -3303,7 +3306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C58">
         <v>0</v>
       </c>
@@ -3338,42 +3341,42 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="C59" s="17">
-        <v>1</v>
-      </c>
-      <c r="D59" s="17">
-        <v>1</v>
-      </c>
-      <c r="E59" s="17">
-        <v>1</v>
-      </c>
-      <c r="F59" s="17">
-        <v>1</v>
-      </c>
-      <c r="G59" s="17">
-        <v>1</v>
-      </c>
-      <c r="H59" s="17">
-        <v>0</v>
-      </c>
-      <c r="I59" s="17">
-        <v>0</v>
-      </c>
-      <c r="J59" s="17">
-        <v>1</v>
-      </c>
-      <c r="K59" s="17">
-        <v>0</v>
-      </c>
-      <c r="L59" s="17">
-        <v>1</v>
-      </c>
-      <c r="M59" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="C59" s="15">
+        <v>1</v>
+      </c>
+      <c r="D59" s="15">
+        <v>1</v>
+      </c>
+      <c r="E59" s="15">
+        <v>1</v>
+      </c>
+      <c r="F59" s="15">
+        <v>1</v>
+      </c>
+      <c r="G59" s="15">
+        <v>1</v>
+      </c>
+      <c r="H59" s="15">
+        <v>0</v>
+      </c>
+      <c r="I59" s="15">
+        <v>0</v>
+      </c>
+      <c r="J59" s="15">
+        <v>1</v>
+      </c>
+      <c r="K59" s="15">
+        <v>0</v>
+      </c>
+      <c r="L59" s="15">
+        <v>1</v>
+      </c>
+      <c r="M59" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C61">
         <v>0</v>
       </c>
@@ -3392,174 +3395,174 @@
       <c r="H61">
         <v>0</v>
       </c>
-      <c r="I61" s="18">
-        <v>1</v>
-      </c>
-      <c r="J61" s="18">
-        <v>1</v>
-      </c>
-      <c r="K61" s="18">
-        <v>1</v>
-      </c>
-      <c r="L61" s="18">
-        <v>1</v>
-      </c>
-      <c r="M61" s="18">
-        <v>0</v>
-      </c>
-      <c r="N61" s="18">
-        <v>0</v>
-      </c>
-      <c r="O61" s="18">
-        <v>1</v>
-      </c>
-      <c r="P61" s="18">
-        <v>0</v>
-      </c>
-      <c r="Q61" s="18">
-        <v>1</v>
-      </c>
-      <c r="R61" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="C62" s="14">
+      <c r="I61" s="16">
+        <v>1</v>
+      </c>
+      <c r="J61" s="16">
+        <v>1</v>
+      </c>
+      <c r="K61" s="16">
+        <v>1</v>
+      </c>
+      <c r="L61" s="16">
+        <v>1</v>
+      </c>
+      <c r="M61" s="16">
+        <v>0</v>
+      </c>
+      <c r="N61" s="16">
+        <v>0</v>
+      </c>
+      <c r="O61" s="16">
+        <v>1</v>
+      </c>
+      <c r="P61" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q61" s="16">
+        <v>1</v>
+      </c>
+      <c r="R61" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="C62" s="20">
         <v>3</v>
       </c>
-      <c r="D62" s="14"/>
-      <c r="E62" s="14"/>
-      <c r="F62" s="14"/>
-      <c r="G62" s="14" t="s">
+      <c r="D62" s="20"/>
+      <c r="E62" s="20"/>
+      <c r="F62" s="20"/>
+      <c r="G62" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="H62" s="14"/>
-      <c r="I62" s="14"/>
-      <c r="J62" s="14"/>
-      <c r="K62" s="14" t="s">
+      <c r="H62" s="20"/>
+      <c r="I62" s="20"/>
+      <c r="J62" s="20"/>
+      <c r="K62" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="L62" s="14"/>
-      <c r="M62" s="14"/>
-      <c r="N62" s="14"/>
-      <c r="O62" s="14" t="s">
+      <c r="L62" s="20"/>
+      <c r="M62" s="20"/>
+      <c r="N62" s="20"/>
+      <c r="O62" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="P62" s="20"/>
+      <c r="Q62" s="20"/>
+      <c r="R62" s="20"/>
+    </row>
+    <row r="64" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B64" t="s">
+        <v>126</v>
+      </c>
+      <c r="C64">
+        <v>1</v>
+      </c>
+      <c r="D64" s="7">
+        <v>1</v>
+      </c>
+      <c r="E64" s="7">
+        <v>0</v>
+      </c>
+      <c r="F64" s="7">
+        <v>0</v>
+      </c>
+      <c r="G64" s="7">
+        <v>1</v>
+      </c>
+      <c r="H64" s="7">
+        <v>0</v>
+      </c>
+      <c r="I64" s="7">
+        <v>0</v>
+      </c>
+      <c r="J64" s="7">
+        <v>1</v>
+      </c>
+      <c r="K64" s="7">
+        <v>0</v>
+      </c>
+      <c r="L64" s="7">
+        <v>0</v>
+      </c>
+      <c r="M64" s="7">
+        <v>0</v>
+      </c>
+      <c r="N64" s="7">
+        <v>0</v>
+      </c>
+      <c r="O64" s="7"/>
+    </row>
+    <row r="65" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B65" t="s">
+        <v>128</v>
+      </c>
+      <c r="C65" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="D65" s="20"/>
+      <c r="E65" s="20"/>
+      <c r="F65" s="20"/>
+      <c r="G65" s="20">
+        <v>9</v>
+      </c>
+      <c r="H65" s="20"/>
+      <c r="I65" s="20"/>
+      <c r="J65" s="20"/>
+      <c r="K65" s="20">
+        <v>0</v>
+      </c>
+      <c r="L65" s="20"/>
+      <c r="M65" s="20"/>
+      <c r="N65" s="20"/>
+    </row>
+    <row r="66" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B66" t="s">
         <v>125</v>
       </c>
-      <c r="P62" s="14"/>
-      <c r="Q62" s="14"/>
-      <c r="R62" s="14"/>
-    </row>
-    <row r="64" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="B64" t="s">
-        <v>127</v>
-      </c>
-      <c r="C64">
-        <v>1</v>
-      </c>
-      <c r="D64" s="7">
-        <v>1</v>
-      </c>
-      <c r="E64" s="7">
-        <v>0</v>
-      </c>
-      <c r="F64" s="7">
-        <v>0</v>
-      </c>
-      <c r="G64" s="7">
-        <v>1</v>
-      </c>
-      <c r="H64" s="7">
-        <v>0</v>
-      </c>
-      <c r="I64" s="7">
-        <v>0</v>
-      </c>
-      <c r="J64" s="7">
-        <v>1</v>
-      </c>
-      <c r="K64" s="7">
-        <v>0</v>
-      </c>
-      <c r="L64" s="7">
-        <v>0</v>
-      </c>
-      <c r="M64" s="7">
-        <v>0</v>
-      </c>
-      <c r="N64" s="7">
-        <v>0</v>
-      </c>
-      <c r="O64" s="7"/>
-    </row>
-    <row r="65" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="B65" t="s">
-        <v>129</v>
-      </c>
-      <c r="C65" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="D65" s="14"/>
-      <c r="E65" s="14"/>
-      <c r="F65" s="14"/>
-      <c r="G65" s="14">
-        <v>9</v>
-      </c>
-      <c r="H65" s="14"/>
-      <c r="I65" s="14"/>
-      <c r="J65" s="14"/>
-      <c r="K65" s="14">
-        <v>0</v>
-      </c>
-      <c r="L65" s="14"/>
-      <c r="M65" s="14"/>
-      <c r="N65" s="14"/>
-    </row>
-    <row r="66" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="B66" t="s">
-        <v>126</v>
-      </c>
-      <c r="C66" s="19">
-        <v>0</v>
-      </c>
-      <c r="D66" s="19">
-        <v>0</v>
-      </c>
-      <c r="E66" s="19">
-        <v>0</v>
-      </c>
-      <c r="F66" s="19">
-        <v>1</v>
-      </c>
-      <c r="G66" s="20">
-        <v>0</v>
-      </c>
-      <c r="H66" s="20">
-        <v>1</v>
-      </c>
-      <c r="I66" s="20">
-        <v>0</v>
-      </c>
-      <c r="J66" s="20">
-        <v>1</v>
-      </c>
-      <c r="K66" s="20">
-        <v>0</v>
-      </c>
-      <c r="L66" s="20">
-        <v>1</v>
-      </c>
-      <c r="M66" s="20">
-        <v>0</v>
-      </c>
-      <c r="N66" s="22">
+      <c r="C66" s="17">
+        <v>0</v>
+      </c>
+      <c r="D66" s="17">
+        <v>0</v>
+      </c>
+      <c r="E66" s="17">
+        <v>0</v>
+      </c>
+      <c r="F66" s="17">
+        <v>1</v>
+      </c>
+      <c r="G66" s="18">
+        <v>0</v>
+      </c>
+      <c r="H66" s="18">
+        <v>1</v>
+      </c>
+      <c r="I66" s="18">
+        <v>0</v>
+      </c>
+      <c r="J66" s="18">
+        <v>1</v>
+      </c>
+      <c r="K66" s="18">
+        <v>0</v>
+      </c>
+      <c r="L66" s="18">
+        <v>1</v>
+      </c>
+      <c r="M66" s="18">
+        <v>0</v>
+      </c>
+      <c r="N66" s="19">
         <v>0</v>
       </c>
       <c r="O66" s="7"/>
       <c r="P66" s="7"/>
     </row>
-    <row r="67" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C67" s="21">
         <v>1</v>
@@ -3573,26 +3576,26 @@
       <c r="H67" s="21"/>
       <c r="I67" s="21"/>
       <c r="J67" s="21"/>
-      <c r="K67" s="14">
+      <c r="K67" s="20">
         <v>4</v>
       </c>
-      <c r="L67" s="14"/>
-      <c r="M67" s="14"/>
-      <c r="N67" s="14"/>
-    </row>
-    <row r="69" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="L67" s="20"/>
+      <c r="M67" s="20"/>
+      <c r="N67" s="20"/>
+    </row>
+    <row r="69" spans="2:18" x14ac:dyDescent="0.3">
       <c r="E69" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="70" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="70" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="71" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="71" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B71" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C71" s="6">
         <v>0</v>
@@ -3643,25 +3646,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="C72" s="14"/>
-      <c r="D72" s="14"/>
-      <c r="E72" s="14"/>
-      <c r="F72" s="14"/>
-      <c r="G72" s="14"/>
-      <c r="H72" s="14"/>
-      <c r="I72" s="14"/>
-      <c r="J72" s="14"/>
-      <c r="K72" s="14"/>
-      <c r="L72" s="14"/>
-      <c r="M72" s="14"/>
-      <c r="N72" s="14"/>
-      <c r="O72" s="14"/>
-      <c r="P72" s="14"/>
-      <c r="Q72" s="14"/>
-      <c r="R72" s="14"/>
-    </row>
-    <row r="73" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="C72" s="20"/>
+      <c r="D72" s="20"/>
+      <c r="E72" s="20"/>
+      <c r="F72" s="20"/>
+      <c r="G72" s="20"/>
+      <c r="H72" s="20"/>
+      <c r="I72" s="20"/>
+      <c r="J72" s="20"/>
+      <c r="K72" s="20"/>
+      <c r="L72" s="20"/>
+      <c r="M72" s="20"/>
+      <c r="N72" s="20"/>
+      <c r="O72" s="20"/>
+      <c r="P72" s="20"/>
+      <c r="Q72" s="20"/>
+      <c r="R72" s="20"/>
+    </row>
+    <row r="73" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B73" t="s">
         <v>116</v>
       </c>
@@ -3714,9 +3717,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B75" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C75">
         <v>1</v>
@@ -3755,29 +3758,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="C76" s="14" t="s">
+    <row r="76" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="C76" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="D76" s="14"/>
-      <c r="E76" s="14"/>
-      <c r="F76" s="14"/>
-      <c r="G76" s="14">
+      <c r="D76" s="20"/>
+      <c r="E76" s="20"/>
+      <c r="F76" s="20"/>
+      <c r="G76" s="20">
         <v>9</v>
       </c>
-      <c r="H76" s="14"/>
-      <c r="I76" s="14"/>
-      <c r="J76" s="14"/>
-      <c r="K76" s="14">
-        <v>0</v>
-      </c>
-      <c r="L76" s="14"/>
-      <c r="M76" s="14"/>
-      <c r="N76" s="14"/>
-    </row>
-    <row r="77" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="H76" s="20"/>
+      <c r="I76" s="20"/>
+      <c r="J76" s="20"/>
+      <c r="K76" s="20">
+        <v>0</v>
+      </c>
+      <c r="L76" s="20"/>
+      <c r="M76" s="20"/>
+      <c r="N76" s="20"/>
+    </row>
+    <row r="77" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B77" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C77">
         <v>0</v>
@@ -3816,140 +3819,140 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="C78" s="14">
+    <row r="78" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="C78" s="20">
         <v>2</v>
       </c>
-      <c r="D78" s="14"/>
-      <c r="E78" s="14"/>
-      <c r="F78" s="14"/>
-      <c r="G78" s="14">
-        <v>1</v>
-      </c>
-      <c r="H78" s="14"/>
-      <c r="I78" s="14"/>
-      <c r="J78" s="14"/>
-      <c r="K78" s="14">
+      <c r="D78" s="20"/>
+      <c r="E78" s="20"/>
+      <c r="F78" s="20"/>
+      <c r="G78" s="20">
+        <v>1</v>
+      </c>
+      <c r="H78" s="20"/>
+      <c r="I78" s="20"/>
+      <c r="J78" s="20"/>
+      <c r="K78" s="20">
         <v>4</v>
       </c>
-      <c r="L78" s="14"/>
-      <c r="M78" s="14"/>
-      <c r="N78" s="14"/>
-    </row>
-    <row r="80" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="L78" s="20"/>
+      <c r="M78" s="20"/>
+      <c r="N78" s="20"/>
+    </row>
+    <row r="80" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C80" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="81" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="C81" s="20">
+        <v>1</v>
+      </c>
+      <c r="D81" s="20"/>
+      <c r="E81" s="20"/>
+      <c r="F81" s="20"/>
+      <c r="G81" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="H81" s="20"/>
+      <c r="I81" s="20"/>
+      <c r="J81" s="20"/>
+      <c r="K81" s="20">
+        <v>1</v>
+      </c>
+      <c r="L81" s="20"/>
+      <c r="M81" s="20"/>
+      <c r="N81" s="20"/>
+      <c r="O81" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="P81" s="20"/>
+      <c r="Q81" s="20"/>
+      <c r="R81" s="20"/>
+      <c r="S81" s="20">
+        <v>4</v>
+      </c>
+      <c r="T81" s="20"/>
+      <c r="U81" s="20"/>
+      <c r="V81" s="20"/>
+    </row>
+    <row r="82" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="C82">
+        <v>0</v>
+      </c>
+      <c r="D82">
+        <v>0</v>
+      </c>
+      <c r="E82">
+        <v>0</v>
+      </c>
+      <c r="F82">
+        <v>1</v>
+      </c>
+      <c r="G82">
+        <v>1</v>
+      </c>
+      <c r="H82">
+        <v>0</v>
+      </c>
+      <c r="I82">
+        <v>1</v>
+      </c>
+      <c r="J82">
+        <v>0</v>
+      </c>
+      <c r="K82">
+        <v>0</v>
+      </c>
+      <c r="L82">
+        <v>0</v>
+      </c>
+      <c r="M82">
+        <v>0</v>
+      </c>
+      <c r="N82">
+        <v>1</v>
+      </c>
+      <c r="O82">
+        <v>1</v>
+      </c>
+      <c r="P82">
+        <v>0</v>
+      </c>
+      <c r="Q82">
+        <v>1</v>
+      </c>
+      <c r="R82">
+        <v>1</v>
+      </c>
+      <c r="S82">
+        <v>0</v>
+      </c>
+      <c r="T82">
+        <v>1</v>
+      </c>
+      <c r="U82">
+        <v>0</v>
+      </c>
+      <c r="V82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="C84" s="20" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="81" spans="2:22" x14ac:dyDescent="0.55000000000000004">
-      <c r="C81" s="14">
-        <v>1</v>
-      </c>
-      <c r="D81" s="14"/>
-      <c r="E81" s="14"/>
-      <c r="F81" s="14"/>
-      <c r="G81" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="H81" s="14"/>
-      <c r="I81" s="14"/>
-      <c r="J81" s="14"/>
-      <c r="K81" s="14">
-        <v>1</v>
-      </c>
-      <c r="L81" s="14"/>
-      <c r="M81" s="14"/>
-      <c r="N81" s="14"/>
-      <c r="O81" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="P81" s="14"/>
-      <c r="Q81" s="14"/>
-      <c r="R81" s="14"/>
-      <c r="S81" s="14">
-        <v>4</v>
-      </c>
-      <c r="T81" s="14"/>
-      <c r="U81" s="14"/>
-      <c r="V81" s="14"/>
-    </row>
-    <row r="82" spans="2:22" x14ac:dyDescent="0.55000000000000004">
-      <c r="C82">
-        <v>0</v>
-      </c>
-      <c r="D82">
-        <v>0</v>
-      </c>
-      <c r="E82">
-        <v>0</v>
-      </c>
-      <c r="F82">
-        <v>1</v>
-      </c>
-      <c r="G82">
-        <v>1</v>
-      </c>
-      <c r="H82">
-        <v>0</v>
-      </c>
-      <c r="I82">
-        <v>1</v>
-      </c>
-      <c r="J82">
-        <v>0</v>
-      </c>
-      <c r="K82">
-        <v>0</v>
-      </c>
-      <c r="L82">
-        <v>0</v>
-      </c>
-      <c r="M82">
-        <v>0</v>
-      </c>
-      <c r="N82">
-        <v>1</v>
-      </c>
-      <c r="O82">
-        <v>1</v>
-      </c>
-      <c r="P82">
-        <v>0</v>
-      </c>
-      <c r="Q82">
-        <v>1</v>
-      </c>
-      <c r="R82">
-        <v>1</v>
-      </c>
-      <c r="S82">
-        <v>0</v>
-      </c>
-      <c r="T82">
-        <v>1</v>
-      </c>
-      <c r="U82">
-        <v>0</v>
-      </c>
-      <c r="V82">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="2:22" x14ac:dyDescent="0.55000000000000004">
-      <c r="C84" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="D84" s="14"/>
-      <c r="E84" s="14"/>
-      <c r="F84" s="14"/>
-      <c r="G84" s="14"/>
-      <c r="H84" s="14"/>
-      <c r="I84" s="14"/>
-      <c r="J84" s="14"/>
-      <c r="K84" s="14"/>
-      <c r="L84" s="14"/>
-    </row>
-    <row r="85" spans="2:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="D84" s="20"/>
+      <c r="E84" s="20"/>
+      <c r="F84" s="20"/>
+      <c r="G84" s="20"/>
+      <c r="H84" s="20"/>
+      <c r="I84" s="20"/>
+      <c r="J84" s="20"/>
+      <c r="K84" s="20"/>
+      <c r="L84" s="20"/>
+    </row>
+    <row r="85" spans="2:22" x14ac:dyDescent="0.3">
       <c r="C85">
         <v>1</v>
       </c>
@@ -3981,33 +3984,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="2:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="2:22" x14ac:dyDescent="0.3">
       <c r="C86" s="7"/>
       <c r="D86" s="7"/>
-      <c r="E86" s="14">
+      <c r="E86" s="20">
         <v>8</v>
       </c>
-      <c r="F86" s="14"/>
-      <c r="G86" s="14"/>
-      <c r="H86" s="14"/>
-      <c r="I86" s="14">
+      <c r="F86" s="20"/>
+      <c r="G86" s="20"/>
+      <c r="H86" s="20"/>
+      <c r="I86" s="20">
         <v>6</v>
       </c>
-      <c r="J86" s="14"/>
-      <c r="K86" s="14"/>
-      <c r="L86" s="14"/>
-    </row>
-    <row r="87" spans="2:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="J86" s="20"/>
+      <c r="K86" s="20"/>
+      <c r="L86" s="20"/>
+    </row>
+    <row r="87" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B87" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="89" spans="2:22" x14ac:dyDescent="0.55000000000000004">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="89" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B89" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="90" spans="2:22" x14ac:dyDescent="0.55000000000000004">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="90" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B90" t="s">
         <v>119</v>
       </c>
@@ -4060,7 +4063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="2:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B92" t="s">
         <v>123</v>
       </c>
@@ -4113,7 +4116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="2:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="2:22" x14ac:dyDescent="0.3">
       <c r="C94">
         <v>1</v>
       </c>
@@ -4151,27 +4154,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="2:22" x14ac:dyDescent="0.55000000000000004">
-      <c r="C95" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="D95" s="14"/>
-      <c r="E95" s="14"/>
-      <c r="F95" s="14"/>
-      <c r="G95" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="H95" s="14"/>
-      <c r="I95" s="14"/>
-      <c r="J95" s="14"/>
-      <c r="K95" s="14">
+    <row r="95" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="C95" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="D95" s="20"/>
+      <c r="E95" s="20"/>
+      <c r="F95" s="20"/>
+      <c r="G95" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="H95" s="20"/>
+      <c r="I95" s="20"/>
+      <c r="J95" s="20"/>
+      <c r="K95" s="20">
         <v>6</v>
       </c>
-      <c r="L95" s="14"/>
-      <c r="M95" s="14"/>
-      <c r="N95" s="14"/>
-    </row>
-    <row r="96" spans="2:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="L95" s="20"/>
+      <c r="M95" s="20"/>
+      <c r="N95" s="20"/>
+    </row>
+    <row r="96" spans="2:22" x14ac:dyDescent="0.3">
       <c r="C96">
         <v>0</v>
       </c>
@@ -4209,33 +4212,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="C97" s="14">
-        <v>1</v>
-      </c>
-      <c r="D97" s="14"/>
-      <c r="E97" s="14"/>
-      <c r="F97" s="14"/>
-      <c r="G97" s="14">
-        <v>0</v>
-      </c>
-      <c r="H97" s="14"/>
-      <c r="I97" s="14"/>
-      <c r="J97" s="14"/>
-      <c r="K97" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="L97" s="14"/>
-      <c r="M97" s="14"/>
-      <c r="N97" s="14"/>
-    </row>
-    <row r="98" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="C97" s="20">
+        <v>1</v>
+      </c>
+      <c r="D97" s="20"/>
+      <c r="E97" s="20"/>
+      <c r="F97" s="20"/>
+      <c r="G97" s="20">
+        <v>0</v>
+      </c>
+      <c r="H97" s="20"/>
+      <c r="I97" s="20"/>
+      <c r="J97" s="20"/>
+      <c r="K97" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="L97" s="20"/>
+      <c r="M97" s="20"/>
+      <c r="N97" s="20"/>
+    </row>
+    <row r="98" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B98" t="s">
         <v>112</v>
       </c>
-      <c r="C98">
-        <v>1</v>
-      </c>
       <c r="D98">
         <v>1</v>
       </c>
@@ -4266,10 +4266,33 @@
       <c r="M98">
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="N98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="C99" s="20">
+        <v>7</v>
+      </c>
+      <c r="D99" s="20"/>
+      <c r="E99" s="20"/>
+      <c r="F99" s="20"/>
+      <c r="G99" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="H99" s="20"/>
+      <c r="I99" s="20"/>
+      <c r="J99" s="20"/>
+      <c r="K99" s="20">
+        <v>4</v>
+      </c>
+      <c r="L99" s="20"/>
+      <c r="M99" s="20"/>
+      <c r="N99" s="20"/>
+    </row>
+    <row r="100" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B100" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C100">
         <v>0</v>
@@ -4320,34 +4343,136 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="C101" s="14">
+    <row r="101" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="C101" s="20">
         <v>3</v>
       </c>
-      <c r="D101" s="14"/>
-      <c r="E101" s="14"/>
-      <c r="F101" s="14"/>
-      <c r="G101" s="14" t="s">
+      <c r="D101" s="20"/>
+      <c r="E101" s="20"/>
+      <c r="F101" s="20"/>
+      <c r="G101" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="H101" s="14"/>
-      <c r="I101" s="14"/>
-      <c r="J101" s="14"/>
-      <c r="K101" s="14" t="s">
+      <c r="H101" s="20"/>
+      <c r="I101" s="20"/>
+      <c r="J101" s="20"/>
+      <c r="K101" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="L101" s="14"/>
-      <c r="M101" s="14"/>
-      <c r="N101" s="14"/>
-      <c r="O101" s="14">
+      <c r="L101" s="20"/>
+      <c r="M101" s="20"/>
+      <c r="N101" s="20"/>
+      <c r="O101" s="20">
         <v>5</v>
       </c>
-      <c r="P101" s="14"/>
-      <c r="Q101" s="14"/>
-      <c r="R101" s="14"/>
+      <c r="P101" s="20"/>
+      <c r="Q101" s="20"/>
+      <c r="R101" s="20"/>
+    </row>
+    <row r="103" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="C103">
+        <v>1</v>
+      </c>
+      <c r="D103">
+        <v>0</v>
+      </c>
+      <c r="E103">
+        <v>0</v>
+      </c>
+      <c r="F103">
+        <v>0</v>
+      </c>
+      <c r="G103">
+        <v>0</v>
+      </c>
+      <c r="H103">
+        <v>1</v>
+      </c>
+      <c r="I103">
+        <v>1</v>
+      </c>
+      <c r="J103">
+        <v>1</v>
+      </c>
+      <c r="K103">
+        <v>0</v>
+      </c>
+      <c r="L103">
+        <v>0</v>
+      </c>
+      <c r="M103">
+        <v>0</v>
+      </c>
+      <c r="N103">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="74">
+  <mergeCells count="77">
+    <mergeCell ref="O35:R35"/>
+    <mergeCell ref="C37:F37"/>
+    <mergeCell ref="G37:J37"/>
+    <mergeCell ref="K37:N37"/>
+    <mergeCell ref="O37:R37"/>
+    <mergeCell ref="C35:F35"/>
+    <mergeCell ref="G35:J35"/>
+    <mergeCell ref="K35:N35"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="N2:R2"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="K3:N3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="A8:V8"/>
+    <mergeCell ref="A26:S26"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="M4:P4"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="K6:P6"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="I5:R5"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="C51:F51"/>
+    <mergeCell ref="G51:J51"/>
+    <mergeCell ref="K51:N51"/>
+    <mergeCell ref="O51:R51"/>
+    <mergeCell ref="C62:F62"/>
+    <mergeCell ref="G62:J62"/>
+    <mergeCell ref="K62:N62"/>
+    <mergeCell ref="O62:R62"/>
+    <mergeCell ref="C65:F65"/>
+    <mergeCell ref="G65:J65"/>
+    <mergeCell ref="K65:N65"/>
+    <mergeCell ref="C67:F67"/>
+    <mergeCell ref="G67:J67"/>
+    <mergeCell ref="K67:N67"/>
+    <mergeCell ref="C72:F72"/>
+    <mergeCell ref="G72:J72"/>
+    <mergeCell ref="K72:N72"/>
+    <mergeCell ref="O72:R72"/>
+    <mergeCell ref="C76:F76"/>
+    <mergeCell ref="G76:J76"/>
+    <mergeCell ref="K76:N76"/>
+    <mergeCell ref="C78:F78"/>
+    <mergeCell ref="G78:J78"/>
+    <mergeCell ref="K78:N78"/>
+    <mergeCell ref="C81:F81"/>
+    <mergeCell ref="G81:J81"/>
+    <mergeCell ref="K81:N81"/>
+    <mergeCell ref="O81:R81"/>
+    <mergeCell ref="S81:V81"/>
+    <mergeCell ref="I86:L86"/>
+    <mergeCell ref="C84:L84"/>
+    <mergeCell ref="E86:H86"/>
     <mergeCell ref="C101:F101"/>
     <mergeCell ref="G101:J101"/>
     <mergeCell ref="K101:N101"/>
@@ -4358,70 +4483,9 @@
     <mergeCell ref="C97:F97"/>
     <mergeCell ref="G97:J97"/>
     <mergeCell ref="K97:N97"/>
-    <mergeCell ref="O81:R81"/>
-    <mergeCell ref="S81:V81"/>
-    <mergeCell ref="I86:L86"/>
-    <mergeCell ref="C84:L84"/>
-    <mergeCell ref="E86:H86"/>
-    <mergeCell ref="C78:F78"/>
-    <mergeCell ref="G78:J78"/>
-    <mergeCell ref="K78:N78"/>
-    <mergeCell ref="C81:F81"/>
-    <mergeCell ref="G81:J81"/>
-    <mergeCell ref="K81:N81"/>
-    <mergeCell ref="C72:F72"/>
-    <mergeCell ref="G72:J72"/>
-    <mergeCell ref="K72:N72"/>
-    <mergeCell ref="O72:R72"/>
-    <mergeCell ref="C76:F76"/>
-    <mergeCell ref="G76:J76"/>
-    <mergeCell ref="K76:N76"/>
-    <mergeCell ref="C65:F65"/>
-    <mergeCell ref="G65:J65"/>
-    <mergeCell ref="K65:N65"/>
-    <mergeCell ref="C67:F67"/>
-    <mergeCell ref="G67:J67"/>
-    <mergeCell ref="K67:N67"/>
-    <mergeCell ref="C51:F51"/>
-    <mergeCell ref="G51:J51"/>
-    <mergeCell ref="K51:N51"/>
-    <mergeCell ref="O51:R51"/>
-    <mergeCell ref="C62:F62"/>
-    <mergeCell ref="G62:J62"/>
-    <mergeCell ref="K62:N62"/>
-    <mergeCell ref="O62:R62"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="M4:P4"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="K6:P6"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="I5:R5"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="A8:V8"/>
-    <mergeCell ref="A26:S26"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="N2:R2"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="K3:N3"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="O35:R35"/>
-    <mergeCell ref="C37:F37"/>
-    <mergeCell ref="G37:J37"/>
-    <mergeCell ref="K37:N37"/>
-    <mergeCell ref="O37:R37"/>
-    <mergeCell ref="C35:F35"/>
-    <mergeCell ref="G35:J35"/>
-    <mergeCell ref="K35:N35"/>
+    <mergeCell ref="C99:F99"/>
+    <mergeCell ref="G99:J99"/>
+    <mergeCell ref="K99:N99"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4437,62 +4501,62 @@
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="19.68359375" customWidth="1"/>
-    <col min="3" max="3" width="12.5234375" customWidth="1"/>
-    <col min="4" max="36" width="4.68359375" customWidth="1"/>
-    <col min="37" max="37" width="4.3125" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" customWidth="1"/>
+    <col min="4" max="36" width="4.6640625" customWidth="1"/>
+    <col min="37" max="37" width="4.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15"/>
-      <c r="W1" s="15"/>
-      <c r="X1" s="15"/>
-      <c r="Y1" s="15"/>
-      <c r="Z1" s="15"/>
-      <c r="AA1" s="15"/>
-      <c r="AB1" s="15"/>
-      <c r="AC1" s="15"/>
-      <c r="AD1" s="15"/>
-      <c r="AE1" s="15"/>
-      <c r="AF1" s="15"/>
-      <c r="AG1" s="15"/>
-      <c r="AH1" s="15"/>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="22"/>
+      <c r="AB1" s="22"/>
+      <c r="AC1" s="22"/>
+      <c r="AD1" s="22"/>
+      <c r="AE1" s="22"/>
+      <c r="AF1" s="22"/>
+      <c r="AG1" s="22"/>
+      <c r="AH1" s="22"/>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
       <c r="D2">
         <v>0</v>
       </c>
@@ -4587,7 +4651,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -4609,7 +4673,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -4631,7 +4695,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -4656,7 +4720,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -4681,7 +4745,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -4706,7 +4770,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -4731,7 +4795,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -4753,7 +4817,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -4778,7 +4842,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -4803,7 +4867,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -4828,7 +4892,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -4853,7 +4917,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -4878,7 +4942,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -4903,7 +4967,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -4928,7 +4992,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>45</v>
       </c>
@@ -4950,7 +5014,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>46</v>
       </c>
@@ -4975,7 +5039,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>35</v>
       </c>

</xml_diff>